<commit_message>
Lowells data for example
</commit_message>
<xml_diff>
--- a/docs/UCB_Densimeter_fitting/Full_Datasets/Used_in_Calibration_2023/UCB_6-8-23/PseudoVoigt.xlsx
+++ b/docs/UCB_Densimeter_fitting/Full_Datasets/Used_in_Calibration_2023/UCB_6-8-23/PseudoVoigt.xlsx
@@ -620,63 +620,63 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.002613684972816</v>
+        <v>0.9973520204120639</v>
       </c>
       <c r="D2" t="n">
-        <v>4.106642300044373e-05</v>
+        <v>4.969691439133369e-05</v>
       </c>
       <c r="E2" t="n">
-        <v>179.3861732011069</v>
+        <v>282.5764020378726</v>
       </c>
       <c r="F2" t="n">
-        <v>1399.181780393892</v>
+        <v>1399.18178038813</v>
       </c>
       <c r="G2" t="n">
-        <v>1219.795607192785</v>
+        <v>1116.605378350257</v>
       </c>
       <c r="H2" t="n">
-        <v>12400.74204660934</v>
+        <v>12400.74198105815</v>
       </c>
       <c r="I2" t="n">
-        <v>2608.645229619548</v>
+        <v>4087.888743058904</v>
       </c>
       <c r="J2" t="n">
-        <v>61.88927618181661</v>
+        <v>61.88927284178892</v>
       </c>
       <c r="K2" t="n">
-        <v>15.82097698312131</v>
+        <v>11.27181845584035</v>
       </c>
       <c r="L2" t="n">
-        <v>4.106642300044373e-05</v>
+        <v>4.96969143913337e-05</v>
       </c>
       <c r="M2" t="n">
-        <v>0.4415960870088867</v>
+        <v>0.441596158182409</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
         <v>0.0063</v>
       </c>
       <c r="P2" t="n">
-        <v>0.498851881989307</v>
+        <v>0.4988515847758431</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4282492218985965</v>
+        <v>0.4487858101455117</v>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
-        <v>0.003818243445237347</v>
+        <v>0.01255072792365499</v>
       </c>
       <c r="T2" t="n">
-        <v>0.4631822052656638</v>
+        <v>0.2923131503078331</v>
       </c>
       <c r="U2" t="n">
-        <v>1.002557135925651</v>
+        <v>0.997285491298794</v>
       </c>
       <c r="V2" t="n">
-        <v>1.002670240399617</v>
+        <v>0.9974185584022668</v>
       </c>
       <c r="W2" t="n">
-        <v>77.71025316493792</v>
+        <v>73.16109129762927</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -742,63 +742,63 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.002636047415286</v>
+        <v>0.9973638843918695</v>
       </c>
       <c r="D3" t="n">
-        <v>4.103005373390781e-05</v>
+        <v>4.943461771075839e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>179.3821722348655</v>
+        <v>282.5730406962603</v>
       </c>
       <c r="F3" t="n">
-        <v>1399.186713092347</v>
+        <v>1399.186713091324</v>
       </c>
       <c r="G3" t="n">
-        <v>1219.804540857482</v>
+        <v>1116.613672395064</v>
       </c>
       <c r="H3" t="n">
-        <v>11791.86939056296</v>
+        <v>11791.86922669792</v>
       </c>
       <c r="I3" t="n">
-        <v>2546.793650364512</v>
+        <v>4136.27448377201</v>
       </c>
       <c r="J3" t="n">
-        <v>60.55961712769042</v>
+        <v>60.55961346136612</v>
       </c>
       <c r="K3" t="n">
-        <v>14.70219480135337</v>
+        <v>9.722830923066146</v>
       </c>
       <c r="L3" t="n">
-        <v>4.103005373390781e-05</v>
+        <v>4.943461771075839e-05</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4442725104062699</v>
+        <v>0.4442725144561843</v>
       </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="n">
         <v>0.00643</v>
       </c>
       <c r="P3" t="n">
-        <v>0.499952752939429</v>
+        <v>0.499952696862576</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.4243493860245897</v>
+        <v>0.4450867738716393</v>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
-        <v>0.003581282681211861</v>
+        <v>0.01240100780574889</v>
       </c>
       <c r="T3" t="n">
-        <v>0.4632651104370564</v>
+        <v>0.3133569696324933</v>
       </c>
       <c r="U3" t="n">
-        <v>1.002580093623431</v>
+        <v>0.9972974232902859</v>
       </c>
       <c r="V3" t="n">
-        <v>1.002692007453028</v>
+        <v>0.9974303543521391</v>
       </c>
       <c r="W3" t="n">
-        <v>75.26181192904379</v>
+        <v>70.28244438443227</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -864,63 +864,63 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.002588209313914</v>
+        <v>0.9973461595108428</v>
       </c>
       <c r="D4" t="n">
-        <v>4.187069355387884e-05</v>
+        <v>4.96312655553865e-05</v>
       </c>
       <c r="E4" t="n">
-        <v>179.3907313845343</v>
+        <v>282.5780625971117</v>
       </c>
       <c r="F4" t="n">
-        <v>1399.192097159666</v>
+        <v>1399.192097159655</v>
       </c>
       <c r="G4" t="n">
-        <v>1219.801365775132</v>
+        <v>1116.614034562543</v>
       </c>
       <c r="H4" t="n">
-        <v>12012.65724475469</v>
+        <v>12012.65727920115</v>
       </c>
       <c r="I4" t="n">
-        <v>2594.301766967521</v>
+        <v>4051.373774169645</v>
       </c>
       <c r="J4" t="n">
-        <v>61.96330378643245</v>
+        <v>61.96330442919957</v>
       </c>
       <c r="K4" t="n">
-        <v>15.58616025175459</v>
+        <v>11.30907354150381</v>
       </c>
       <c r="L4" t="n">
-        <v>4.187069355387884e-05</v>
+        <v>4.963126555538649e-05</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4430201052753633</v>
+        <v>0.4430201050851046</v>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
         <v>0.00644</v>
       </c>
       <c r="P4" t="n">
-        <v>0.4996338269672837</v>
+        <v>0.4996338360641645</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.4211953259623856</v>
+        <v>0.4502818219734405</v>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
-        <v>0.003865842840125135</v>
+        <v>0.01245868382478346</v>
       </c>
       <c r="T4" t="n">
-        <v>0.5058029655920552</v>
+        <v>0.2739466231992534</v>
       </c>
       <c r="U4" t="n">
-        <v>1.002530614794516</v>
+        <v>0.9972794619439361</v>
       </c>
       <c r="V4" t="n">
-        <v>1.002645810451202</v>
+        <v>0.9974128659997481</v>
       </c>
       <c r="W4" t="n">
-        <v>77.54946403818704</v>
+        <v>73.27237797070339</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
@@ -986,63 +986,63 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.002602911246005</v>
+        <v>0.9973488492797445</v>
       </c>
       <c r="D5" t="n">
-        <v>4.109975603417876e-05</v>
+        <v>4.859929415464578e-05</v>
       </c>
       <c r="E5" t="n">
-        <v>179.3881008412543</v>
+        <v>282.5773005070109</v>
       </c>
       <c r="F5" t="n">
-        <v>1399.193628175058</v>
+        <v>1399.193628174454</v>
       </c>
       <c r="G5" t="n">
-        <v>1219.805527333804</v>
+        <v>1116.616327667443</v>
       </c>
       <c r="H5" t="n">
-        <v>11802.74973273963</v>
+        <v>11802.74976107666</v>
       </c>
       <c r="I5" t="n">
-        <v>2531.43391561523</v>
+        <v>4153.10817521906</v>
       </c>
       <c r="J5" t="n">
-        <v>60.26989230206258</v>
+        <v>60.26989246331013</v>
       </c>
       <c r="K5" t="n">
-        <v>15.08868941506985</v>
+        <v>11.2603338829141</v>
       </c>
       <c r="L5" t="n">
-        <v>4.109975603417876e-05</v>
+        <v>4.859929415464577e-05</v>
       </c>
       <c r="M5" t="n">
-        <v>0.4415880934228822</v>
+        <v>0.4415880924233843</v>
       </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
         <v>0.00637</v>
       </c>
       <c r="P5" t="n">
-        <v>0.5097294551187703</v>
+        <v>0.5097294661577725</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.4244213412364893</v>
+        <v>0.4452370532199176</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="n">
-        <v>0.003712328880044183</v>
+        <v>0.01216634555421203</v>
       </c>
       <c r="T5" t="n">
-        <v>0.4780581982819097</v>
+        <v>0.2835597870511327</v>
       </c>
       <c r="U5" t="n">
-        <v>1.002546564118578</v>
+        <v>0.9972834300466999</v>
       </c>
       <c r="V5" t="n">
-        <v>1.002659264707657</v>
+        <v>0.9974142770960198</v>
       </c>
       <c r="W5" t="n">
-        <v>75.35858171713244</v>
+        <v>71.53022634622423</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
@@ -1108,63 +1108,63 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.002580099480207</v>
+        <v>0.9973343751379473</v>
       </c>
       <c r="D6" t="n">
-        <v>4.121700061244413e-05</v>
+        <v>4.788973473534765e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>179.3921824695906</v>
+        <v>282.5814015026431</v>
       </c>
       <c r="F6" t="n">
-        <v>1399.204967006392</v>
+        <v>1399.204967005978</v>
       </c>
       <c r="G6" t="n">
-        <v>1219.812784536801</v>
+        <v>1116.623565503335</v>
       </c>
       <c r="H6" t="n">
-        <v>11812.2223143384</v>
+        <v>11812.22228973141</v>
       </c>
       <c r="I6" t="n">
-        <v>2598.451104469716</v>
+        <v>4285.193056264594</v>
       </c>
       <c r="J6" t="n">
-        <v>61.58716322702939</v>
+        <v>61.58716265880887</v>
       </c>
       <c r="K6" t="n">
-        <v>14.68110666832906</v>
+        <v>12.04992137715447</v>
       </c>
       <c r="L6" t="n">
-        <v>4.121700061244413e-05</v>
+        <v>4.788973473534764e-05</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4425753582220072</v>
+        <v>0.4425753614292666</v>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
         <v>0.00627</v>
       </c>
       <c r="P6" t="n">
-        <v>0.5108143797872458</v>
+        <v>0.5108143615070191</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.4223897509529218</v>
+        <v>0.4517114362258256</v>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="n">
-        <v>0.003918985811346004</v>
+        <v>0.01199259680598165</v>
       </c>
       <c r="T6" t="n">
-        <v>0.4989172791559172</v>
+        <v>0.2710449352280883</v>
       </c>
       <c r="U6" t="n">
-        <v>1.002523158903972</v>
+        <v>0.9972699238385019</v>
       </c>
       <c r="V6" t="n">
-        <v>1.002637046524947</v>
+        <v>0.9973988347686146</v>
       </c>
       <c r="W6" t="n">
-        <v>76.26826989535846</v>
+        <v>73.63708403596334</v>
       </c>
       <c r="X6" t="inlineStr">
         <is>
@@ -1230,63 +1230,63 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.002588271724025</v>
+        <v>0.9973401245191023</v>
       </c>
       <c r="D7" t="n">
-        <v>4.250952897132289e-05</v>
+        <v>4.737792921001566e-05</v>
       </c>
       <c r="E7" t="n">
-        <v>179.3907202176417</v>
+        <v>282.5797725015184</v>
       </c>
       <c r="F7" t="n">
-        <v>1399.205444926589</v>
+        <v>1399.205444926253</v>
       </c>
       <c r="G7" t="n">
-        <v>1219.814724708947</v>
+        <v>1116.625672424734</v>
       </c>
       <c r="H7" t="n">
-        <v>12041.86652088782</v>
+        <v>12041.86649462387</v>
       </c>
       <c r="I7" t="n">
-        <v>2563.38856849399</v>
+        <v>4318.870362328328</v>
       </c>
       <c r="J7" t="n">
-        <v>62.69997284108149</v>
+        <v>62.69997228707534</v>
       </c>
       <c r="K7" t="n">
-        <v>15.98344469469599</v>
+        <v>13.2806800270088</v>
       </c>
       <c r="L7" t="n">
-        <v>4.250952897132288e-05</v>
+        <v>4.737792921001566e-05</v>
       </c>
       <c r="M7" t="n">
-        <v>0.4434865906270697</v>
+        <v>0.4434865937295057</v>
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
         <v>0.00643</v>
       </c>
       <c r="P7" t="n">
-        <v>0.5092522873227592</v>
+        <v>0.5092522692140466</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.4172072727210349</v>
+        <v>0.4462671280774959</v>
       </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="n">
-        <v>0.0040997749563847</v>
+        <v>0.0117428631262967</v>
       </c>
       <c r="T7" t="n">
-        <v>0.5036833280011063</v>
+        <v>0.3006303649529763</v>
       </c>
       <c r="U7" t="n">
-        <v>1.002529425819242</v>
+        <v>0.9972759891427825</v>
       </c>
       <c r="V7" t="n">
-        <v>1.002647124537421</v>
+        <v>0.9974042681451164</v>
       </c>
       <c r="W7" t="n">
-        <v>78.68341753577748</v>
+        <v>75.98065231408414</v>
       </c>
       <c r="X7" t="inlineStr">
         <is>
@@ -1352,63 +1352,63 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.002575074638198</v>
+        <v>0.9973301074586244</v>
       </c>
       <c r="D8" t="n">
-        <v>4.098036946332272e-05</v>
+        <v>4.689403194396309e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>179.3930815717101</v>
+        <v>282.5826106978686</v>
       </c>
       <c r="F8" t="n">
-        <v>1399.211512464693</v>
+        <v>1399.211512469338</v>
       </c>
       <c r="G8" t="n">
-        <v>1219.818430892983</v>
+        <v>1116.628901771469</v>
       </c>
       <c r="H8" t="n">
-        <v>12120.82154546228</v>
+        <v>12120.82152595241</v>
       </c>
       <c r="I8" t="n">
-        <v>2503.708520602505</v>
+        <v>4372.695117223288</v>
       </c>
       <c r="J8" t="n">
-        <v>61.40430626102928</v>
+        <v>61.40430872492011</v>
       </c>
       <c r="K8" t="n">
-        <v>15.212605771828</v>
+        <v>11.96833152311517</v>
       </c>
       <c r="L8" t="n">
-        <v>4.098036946332273e-05</v>
+        <v>4.689403194396309e-05</v>
       </c>
       <c r="M8" t="n">
-        <v>0.4464873320800677</v>
+        <v>0.4464873298104064</v>
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
         <v>0.00624</v>
       </c>
       <c r="P8" t="n">
-        <v>0.5025513022605748</v>
+        <v>0.5025513047344334</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4330646464838278</v>
+        <v>0.4519614006846209</v>
       </c>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
-        <v>0.003886945528852189</v>
+        <v>0.01169029547740073</v>
       </c>
       <c r="T8" t="n">
-        <v>0.4771888601722212</v>
+        <v>0.2984159598983991</v>
       </c>
       <c r="U8" t="n">
-        <v>1.002518481318305</v>
+        <v>0.9972668293649155</v>
       </c>
       <c r="V8" t="n">
-        <v>1.002631674347967</v>
+        <v>0.9973933935830249</v>
       </c>
       <c r="W8" t="n">
-        <v>76.61691203285727</v>
+        <v>73.37264024803527</v>
       </c>
       <c r="X8" t="inlineStr">
         <is>
@@ -1474,63 +1474,63 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.002574100835638</v>
+        <v>0.99730004789635</v>
       </c>
       <c r="D9" t="n">
-        <v>4.255715541139449e-05</v>
+        <v>4.672392926131259e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>179.3932558166282</v>
+        <v>282.5911280037706</v>
       </c>
       <c r="F9" t="n">
-        <v>1399.224054872771</v>
+        <v>1399.224054871444</v>
       </c>
       <c r="G9" t="n">
-        <v>1219.830799056143</v>
+        <v>1116.632926867674</v>
       </c>
       <c r="H9" t="n">
-        <v>12185.16233346041</v>
+        <v>12185.16235351838</v>
       </c>
       <c r="I9" t="n">
-        <v>2547.837000649892</v>
+        <v>4360.286310568194</v>
       </c>
       <c r="J9" t="n">
-        <v>62.52285277175975</v>
+        <v>62.52285233938186</v>
       </c>
       <c r="K9" t="n">
-        <v>16.49854971518096</v>
+        <v>12.58930296860675</v>
       </c>
       <c r="L9" t="n">
-        <v>4.255715541139449e-05</v>
+        <v>4.672392926131259e-05</v>
       </c>
       <c r="M9" t="n">
-        <v>0.4469409669493892</v>
+        <v>0.4469409692891353</v>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
         <v>0.00639</v>
       </c>
       <c r="P9" t="n">
-        <v>0.5099745565970437</v>
+        <v>0.509974553198882</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.4209243906398288</v>
+        <v>0.4519578932635154</v>
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="n">
-        <v>0.004177676542989523</v>
+        <v>0.01155453963122544</v>
       </c>
       <c r="T9" t="n">
-        <v>0.5039760081695337</v>
+        <v>0.3004509863364854</v>
       </c>
       <c r="U9" t="n">
-        <v>1.002515044798806</v>
+        <v>0.9972367233538193</v>
       </c>
       <c r="V9" t="n">
-        <v>1.002633163830611</v>
+        <v>0.9973633804816096</v>
       </c>
       <c r="W9" t="n">
-        <v>79.0214024869407</v>
+        <v>75.11215530798862</v>
       </c>
       <c r="X9" t="inlineStr">
         <is>
@@ -1596,63 +1596,63 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.002566905632915</v>
+        <v>0.9972957773588904</v>
       </c>
       <c r="D10" t="n">
-        <v>4.202905816329739e-05</v>
+        <v>4.748776120982345e-05</v>
       </c>
       <c r="E10" t="n">
-        <v>179.394543282667</v>
+        <v>282.5923380921167</v>
       </c>
       <c r="F10" t="n">
-        <v>1399.223622311969</v>
+        <v>1399.223622310493</v>
       </c>
       <c r="G10" t="n">
-        <v>1219.829079029302</v>
+        <v>1116.631284218376</v>
       </c>
       <c r="H10" t="n">
-        <v>11912.79430116102</v>
+        <v>11912.79432230535</v>
       </c>
       <c r="I10" t="n">
-        <v>2555.541054403548</v>
+        <v>4408.839042955176</v>
       </c>
       <c r="J10" t="n">
-        <v>62.86195392173533</v>
+        <v>62.86195344495396</v>
       </c>
       <c r="K10" t="n">
-        <v>15.11216812834487</v>
+        <v>12.57959801904356</v>
       </c>
       <c r="L10" t="n">
-        <v>4.202905816329739e-05</v>
+        <v>4.748776120982345e-05</v>
       </c>
       <c r="M10" t="n">
-        <v>0.4437729905679336</v>
+        <v>0.4437729929158654</v>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
         <v>0.00645</v>
       </c>
       <c r="P10" t="n">
-        <v>0.5234299590209716</v>
+        <v>0.5234299559448446</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.4282966169573713</v>
+        <v>0.453902124791588</v>
       </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="n">
-        <v>0.003904591931223229</v>
+        <v>0.01176797533252214</v>
       </c>
       <c r="T10" t="n">
-        <v>0.5027386836176162</v>
+        <v>0.2970989859129086</v>
       </c>
       <c r="U10" t="n">
-        <v>1.002509041152544</v>
+        <v>0.9972314885010216</v>
       </c>
       <c r="V10" t="n">
-        <v>1.002624776793508</v>
+        <v>0.9973600745063566</v>
       </c>
       <c r="W10" t="n">
-        <v>77.9741220500802</v>
+        <v>75.44155146399751</v>
       </c>
       <c r="X10" t="inlineStr">
         <is>
@@ -1718,63 +1718,63 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.002553959392874</v>
+        <v>0.9973067865889192</v>
       </c>
       <c r="D11" t="n">
-        <v>4.27872224670945e-05</v>
+        <v>4.70067368953022e-05</v>
       </c>
       <c r="E11" t="n">
-        <v>179.3968598510648</v>
+        <v>282.5892185665141</v>
       </c>
       <c r="F11" t="n">
-        <v>1399.223440669701</v>
+        <v>1399.223440668404</v>
       </c>
       <c r="G11" t="n">
-        <v>1219.826580818637</v>
+        <v>1116.634222101889</v>
       </c>
       <c r="H11" t="n">
-        <v>12086.62799842913</v>
+        <v>12086.62801199748</v>
       </c>
       <c r="I11" t="n">
-        <v>2669.267055213638</v>
+        <v>4432.393918631524</v>
       </c>
       <c r="J11" t="n">
-        <v>66.20818667774704</v>
+        <v>66.20818617751884</v>
       </c>
       <c r="K11" t="n">
-        <v>15.3640408286908</v>
+        <v>10.70067323119609</v>
       </c>
       <c r="L11" t="n">
-        <v>4.27872224670945e-05</v>
+        <v>4.70067368953022e-05</v>
       </c>
       <c r="M11" t="n">
-        <v>0.4456611839092834</v>
+        <v>0.44566118618364</v>
       </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
         <v>0.00667</v>
       </c>
       <c r="P11" t="n">
-        <v>0.5253006097771517</v>
+        <v>0.5253006050868078</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.4264926793494739</v>
+        <v>0.4528557008495996</v>
       </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
-        <v>0.003798741733335485</v>
+        <v>0.01148760421047739</v>
       </c>
       <c r="T11" t="n">
-        <v>0.4868171042198851</v>
+        <v>0.3078645875735523</v>
       </c>
       <c r="U11" t="n">
-        <v>1.00249545855817</v>
+        <v>0.9972427093445363</v>
       </c>
       <c r="V11" t="n">
-        <v>1.002612467055633</v>
+        <v>0.9973708720683228</v>
       </c>
       <c r="W11" t="n">
-        <v>81.57222750643784</v>
+        <v>76.90885940871493</v>
       </c>
       <c r="X11" t="inlineStr">
         <is>
@@ -1840,63 +1840,63 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1.002705300090321</v>
+        <v>0.9972971197581304</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0001138718505856529</v>
+        <v>4.625640437674619e-05</v>
       </c>
       <c r="E12" t="n">
-        <v>179.3697830560311</v>
+        <v>282.5919577122556</v>
       </c>
       <c r="F12" t="n">
-        <v>1399.217582650957</v>
+        <v>1399.217582650051</v>
       </c>
       <c r="G12" t="n">
-        <v>1219.847799594926</v>
+        <v>1116.625624937795</v>
       </c>
       <c r="H12" t="n">
-        <v>11610.75532208466</v>
+        <v>11610.7553457122</v>
       </c>
       <c r="I12" t="n">
-        <v>3222.169674855181</v>
+        <v>4462.216248167377</v>
       </c>
       <c r="J12" t="n">
-        <v>59.63211382023383</v>
+        <v>59.63211371518476</v>
       </c>
       <c r="K12" t="n">
-        <v>37.3054600733058</v>
+        <v>11.82165249163777</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0001138718505856529</v>
+        <v>4.625640437674619e-05</v>
       </c>
       <c r="M12" t="n">
-        <v>0.4451437477585061</v>
+        <v>0.4451437488737612</v>
       </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
         <v>0.00635</v>
       </c>
       <c r="P12" t="n">
-        <v>0.5159097017163142</v>
+        <v>0.5159097037007931</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.3937195192426857</v>
+        <v>0.4555767296923172</v>
       </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="n">
-        <v>0.01941301198226276</v>
+        <v>0.01142569576695691</v>
       </c>
       <c r="T12" t="n">
-        <v>0.9999999997488338</v>
+        <v>0.3034412112657271</v>
       </c>
       <c r="U12" t="n">
-        <v>1.002561301483738</v>
+        <v>0.9972343913801073</v>
       </c>
       <c r="V12" t="n">
-        <v>1.002849340068096</v>
+        <v>0.9973598560281737</v>
       </c>
       <c r="W12" t="n">
-        <v>96.93757389353962</v>
+        <v>71.45376620682252</v>
       </c>
       <c r="X12" t="inlineStr">
         <is>
@@ -1962,63 +1962,63 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1.002551682225046</v>
+        <v>0.9972912268873316</v>
       </c>
       <c r="D13" t="n">
-        <v>4.088667544431428e-05</v>
+        <v>4.763998142828519e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>179.3972673280707</v>
+        <v>282.5936275132633</v>
       </c>
       <c r="F13" t="n">
-        <v>1399.220686633964</v>
+        <v>1399.220686633032</v>
       </c>
       <c r="G13" t="n">
-        <v>1219.823419305894</v>
+        <v>1116.627059119768</v>
       </c>
       <c r="H13" t="n">
-        <v>11941.725578307</v>
+        <v>11941.72559917746</v>
       </c>
       <c r="I13" t="n">
-        <v>2564.139749991992</v>
+        <v>4324.5987828516</v>
       </c>
       <c r="J13" t="n">
-        <v>60.91988679671183</v>
+        <v>60.91988661065819</v>
       </c>
       <c r="K13" t="n">
-        <v>16.64441825600334</v>
+        <v>11.8770840426474</v>
       </c>
       <c r="L13" t="n">
-        <v>4.088667544431428e-05</v>
+        <v>4.763998142828519e-05</v>
       </c>
       <c r="M13" t="n">
-        <v>0.444652049544263</v>
+        <v>0.4446520507981164</v>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
         <v>0.00621</v>
       </c>
       <c r="P13" t="n">
-        <v>0.5147111178040479</v>
+        <v>0.514711118492413</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.4284059267927478</v>
+        <v>0.452655709394133</v>
       </c>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="n">
-        <v>0.003903524892398618</v>
+        <v>0.01194494356088303</v>
       </c>
       <c r="T13" t="n">
-        <v>0.4915391930336603</v>
+        <v>0.2870982520990891</v>
       </c>
       <c r="U13" t="n">
-        <v>1.002495166537977</v>
+        <v>0.997227161030698</v>
       </c>
       <c r="V13" t="n">
-        <v>1.00260820428462</v>
+        <v>0.9973553009761872</v>
       </c>
       <c r="W13" t="n">
-        <v>77.56430505271517</v>
+        <v>72.79697065330559</v>
       </c>
       <c r="X13" t="inlineStr">
         <is>
@@ -2084,63 +2084,63 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.002538165274582</v>
+        <v>0.9973014617895951</v>
       </c>
       <c r="D14" t="n">
-        <v>4.190564871325105e-05</v>
+        <v>4.684347899273643e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>179.3996860928219</v>
+        <v>282.5907273689552</v>
       </c>
       <c r="F14" t="n">
-        <v>1399.226833419262</v>
+        <v>1399.226833417564</v>
       </c>
       <c r="G14" t="n">
-        <v>1219.827147326441</v>
+        <v>1116.636106048609</v>
       </c>
       <c r="H14" t="n">
-        <v>12239.95365335061</v>
+        <v>12239.95366711978</v>
       </c>
       <c r="I14" t="n">
-        <v>2526.231978723202</v>
+        <v>4390.629146197662</v>
       </c>
       <c r="J14" t="n">
-        <v>63.41213815963985</v>
+        <v>63.41213742559567</v>
       </c>
       <c r="K14" t="n">
-        <v>15.08028848735902</v>
+        <v>12.73141692227285</v>
       </c>
       <c r="L14" t="n">
-        <v>4.190564871325105e-05</v>
+        <v>4.684347899273643e-05</v>
       </c>
       <c r="M14" t="n">
-        <v>0.4418934317244506</v>
+        <v>0.4418934346923539</v>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
         <v>0.00644</v>
       </c>
       <c r="P14" t="n">
-        <v>0.5308407534758155</v>
+        <v>0.5308407463635317</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.4250466579419092</v>
+        <v>0.4526448387542288</v>
       </c>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="n">
-        <v>0.003878739789896316</v>
+        <v>0.01156540853834694</v>
       </c>
       <c r="T14" t="n">
-        <v>0.4994942620699578</v>
+        <v>0.2866084846395912</v>
       </c>
       <c r="U14" t="n">
-        <v>1.002480504440859</v>
+        <v>0.9972379222801144</v>
       </c>
       <c r="V14" t="n">
-        <v>1.002595832741777</v>
+        <v>0.9973650093964944</v>
       </c>
       <c r="W14" t="n">
-        <v>78.49242664699888</v>
+        <v>76.14355434786853</v>
       </c>
       <c r="X14" t="inlineStr">
         <is>
@@ -2206,63 +2206,63 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1.002733194944852</v>
+        <v>0.9972954149118481</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0001588974032684631</v>
+        <v>4.739733204635678e-05</v>
       </c>
       <c r="E15" t="n">
-        <v>179.3647932002741</v>
+        <v>282.5924407946416</v>
       </c>
       <c r="F15" t="n">
-        <v>1399.223566203393</v>
+        <v>1399.223566201592</v>
       </c>
       <c r="G15" t="n">
-        <v>1219.858773003119</v>
+        <v>1116.63112540695</v>
       </c>
       <c r="H15" t="n">
-        <v>11608.22460746277</v>
+        <v>11608.22463653274</v>
       </c>
       <c r="I15" t="n">
-        <v>3063.963284080426</v>
+        <v>4405.567762634019</v>
       </c>
       <c r="J15" t="n">
-        <v>61.97233842148911</v>
+        <v>61.97233791162338</v>
       </c>
       <c r="K15" t="n">
-        <v>40.12734657421406</v>
+        <v>12.69226500986489</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0001588974032684631</v>
+        <v>4.739733204635679e-05</v>
       </c>
       <c r="M15" t="n">
-        <v>0.4421544894056144</v>
+        <v>0.4421544918001505</v>
       </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
         <v>0.00661</v>
       </c>
       <c r="P15" t="n">
-        <v>0.5343723312322975</v>
+        <v>0.5343723301656037</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.3694194473215431</v>
+        <v>0.4552603177269076</v>
       </c>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="n">
-        <v>0.02772349352744769</v>
+        <v>0.01164948746455873</v>
       </c>
       <c r="T15" t="n">
-        <v>0.9999999996211208</v>
+        <v>0.2819955112336252</v>
       </c>
       <c r="U15" t="n">
-        <v>1.002541291370444</v>
+        <v>0.997230979619381</v>
       </c>
       <c r="V15" t="n">
-        <v>1.002925172000588</v>
+        <v>0.9973598585317245</v>
       </c>
       <c r="W15" t="n">
-        <v>102.0996849957032</v>
+        <v>74.66460292148827</v>
       </c>
       <c r="X15" t="inlineStr">
         <is>
@@ -2328,63 +2328,63 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.002512410359093</v>
+        <v>0.9973057223082753</v>
       </c>
       <c r="D16" t="n">
-        <v>4.259733417742839e-05</v>
+        <v>4.850578006369201e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>179.4042949372674</v>
+        <v>282.5895201332542</v>
       </c>
       <c r="F16" t="n">
-        <v>1399.237991608025</v>
+        <v>1399.237991608165</v>
       </c>
       <c r="G16" t="n">
-        <v>1219.833696670757</v>
+        <v>1116.648471474911</v>
       </c>
       <c r="H16" t="n">
-        <v>12211.50260308875</v>
+        <v>12211.5025985104</v>
       </c>
       <c r="I16" t="n">
-        <v>2609.260475146691</v>
+        <v>4364.60872910606</v>
       </c>
       <c r="J16" t="n">
-        <v>63.76441690232266</v>
+        <v>63.76441691638503</v>
       </c>
       <c r="K16" t="n">
-        <v>14.38747571351182</v>
+        <v>13.84711154172536</v>
       </c>
       <c r="L16" t="n">
-        <v>4.259733417742839e-05</v>
+        <v>4.8505780063692e-05</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4414397013867216</v>
+        <v>0.4414397011627023</v>
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
         <v>0.00647</v>
       </c>
       <c r="P16" t="n">
-        <v>0.5367213041277265</v>
+        <v>0.5367213038163581</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.4205193238706856</v>
+        <v>0.4581124363034833</v>
       </c>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
-        <v>0.00406712130155883</v>
+        <v>0.01208416816615732</v>
       </c>
       <c r="T16" t="n">
-        <v>0.5208819578668196</v>
+        <v>0.3044435860585134</v>
       </c>
       <c r="U16" t="n">
-        <v>1.002453532312316</v>
+        <v>0.9972402458418629</v>
       </c>
       <c r="V16" t="n">
-        <v>1.002571295322555</v>
+        <v>0.9973712073733161</v>
       </c>
       <c r="W16" t="n">
-        <v>78.15189261583448</v>
+        <v>77.61152845811039</v>
       </c>
       <c r="X16" t="inlineStr">
         <is>
@@ -2450,63 +2450,63 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1.00252181288649</v>
+        <v>0.997296179471089</v>
       </c>
       <c r="D17" t="n">
-        <v>4.285466547629733e-05</v>
+        <v>4.77464293650123e-05</v>
       </c>
       <c r="E17" t="n">
-        <v>179.4026123266981</v>
+        <v>282.5922241502119</v>
       </c>
       <c r="F17" t="n">
-        <v>1399.243120855663</v>
+        <v>1399.243120855637</v>
       </c>
       <c r="G17" t="n">
-        <v>1219.840508528965</v>
+        <v>1116.650896705425</v>
       </c>
       <c r="H17" t="n">
-        <v>12061.55276345627</v>
+        <v>12061.55275240272</v>
       </c>
       <c r="I17" t="n">
-        <v>2643.723077842606</v>
+        <v>4312.397931425139</v>
       </c>
       <c r="J17" t="n">
-        <v>63.68444588416148</v>
+        <v>63.684445722832</v>
       </c>
       <c r="K17" t="n">
-        <v>15.80188943780566</v>
+        <v>11.78949190803532</v>
       </c>
       <c r="L17" t="n">
-        <v>4.285466547629733e-05</v>
+        <v>4.774642936501231e-05</v>
       </c>
       <c r="M17" t="n">
-        <v>0.4444428577874887</v>
+        <v>0.4444428583730871</v>
       </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
         <v>0.00656</v>
       </c>
       <c r="P17" t="n">
-        <v>0.5388377839897457</v>
+        <v>0.5388377793482646</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.4211060732363057</v>
+        <v>0.452228350191162</v>
       </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="n">
-        <v>0.004009416160721921</v>
+        <v>0.01179072658295087</v>
       </c>
       <c r="T17" t="n">
-        <v>0.4994272516248544</v>
+        <v>0.2994334475551614</v>
       </c>
       <c r="U17" t="n">
-        <v>1.002462753289265</v>
+        <v>0.9972314221295783</v>
       </c>
       <c r="V17" t="n">
-        <v>1.002580879443059</v>
+        <v>0.9973609452234571</v>
       </c>
       <c r="W17" t="n">
-        <v>79.48633532196715</v>
+        <v>75.47393763086731</v>
       </c>
       <c r="X17" t="inlineStr">
         <is>
@@ -2572,63 +2572,63 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.002526677743768</v>
+        <v>0.9972807148676196</v>
       </c>
       <c r="D18" t="n">
-        <v>4.257465234860762e-05</v>
+        <v>4.74824412203751e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>179.4017417582397</v>
+        <v>282.5966062430618</v>
       </c>
       <c r="F18" t="n">
-        <v>1399.236738631353</v>
+        <v>1399.236738631383</v>
       </c>
       <c r="G18" t="n">
-        <v>1219.834996873114</v>
+        <v>1116.640132388321</v>
       </c>
       <c r="H18" t="n">
-        <v>11966.55860656893</v>
+        <v>11966.5585971399</v>
       </c>
       <c r="I18" t="n">
-        <v>2639.179879231451</v>
+        <v>4326.803771491455</v>
       </c>
       <c r="J18" t="n">
-        <v>62.40242809359031</v>
+        <v>62.40242798962629</v>
       </c>
       <c r="K18" t="n">
-        <v>13.75491681232061</v>
+        <v>12.70769554232494</v>
       </c>
       <c r="L18" t="n">
-        <v>4.257465234860762e-05</v>
+        <v>4.748244122037509e-05</v>
       </c>
       <c r="M18" t="n">
-        <v>0.4438444946750466</v>
+        <v>0.4438444950822464</v>
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
         <v>0.00655</v>
       </c>
       <c r="P18" t="n">
-        <v>0.5376343417322436</v>
+        <v>0.5376343380182946</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.4201782073771874</v>
+        <v>0.4526246723041308</v>
       </c>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="n">
-        <v>0.003928872182375059</v>
+        <v>0.01171112012025851</v>
       </c>
       <c r="T18" t="n">
-        <v>0.5115901478012439</v>
+        <v>0.2936606244318223</v>
       </c>
       <c r="U18" t="n">
-        <v>1.002468123488776</v>
+        <v>0.9972162757137358</v>
       </c>
       <c r="V18" t="n">
-        <v>1.002585238839479</v>
+        <v>0.9973451623500336</v>
       </c>
       <c r="W18" t="n">
-        <v>76.15734490591092</v>
+        <v>75.11012353195123</v>
       </c>
       <c r="X18" t="inlineStr">
         <is>
@@ -2694,63 +2694,63 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.002576255661564</v>
+        <v>0.9972858096584727</v>
       </c>
       <c r="D19" t="n">
-        <v>4.240343058789967e-05</v>
+        <v>4.931039328179225e-05</v>
       </c>
       <c r="E19" t="n">
-        <v>179.392870248711</v>
+        <v>282.5951625540104</v>
       </c>
       <c r="F19" t="n">
-        <v>1399.240458026172</v>
+        <v>1399.240458026143</v>
       </c>
       <c r="G19" t="n">
-        <v>1219.847587777461</v>
+        <v>1116.645295472132</v>
       </c>
       <c r="H19" t="n">
-        <v>12341.20335574594</v>
+        <v>12341.20334816642</v>
       </c>
       <c r="I19" t="n">
-        <v>2553.102237559934</v>
+        <v>4261.379807456812</v>
       </c>
       <c r="J19" t="n">
-        <v>64.6191295468271</v>
+        <v>64.61912943879629</v>
       </c>
       <c r="K19" t="n">
-        <v>14.21726241514528</v>
+        <v>12.2927651473398</v>
       </c>
       <c r="L19" t="n">
-        <v>4.240343058789967e-05</v>
+        <v>4.931039328179225e-05</v>
       </c>
       <c r="M19" t="n">
-        <v>0.4420997124056446</v>
+        <v>0.4420997128472524</v>
       </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
         <v>0.00658</v>
       </c>
       <c r="P19" t="n">
-        <v>0.5338212423236507</v>
+        <v>0.5338212390098799</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.4281333201479858</v>
+        <v>0.454936030898626</v>
       </c>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="n">
-        <v>0.003816820494526906</v>
+        <v>0.01228350282851129</v>
       </c>
       <c r="T19" t="n">
-        <v>0.4836715864474751</v>
+        <v>0.3044979388504679</v>
       </c>
       <c r="U19" t="n">
-        <v>1.002518154125665</v>
+        <v>0.9972192443009292</v>
       </c>
       <c r="V19" t="n">
-        <v>1.002634363932472</v>
+        <v>0.9973523839032147</v>
       </c>
       <c r="W19" t="n">
-        <v>78.83639196197238</v>
+        <v>76.9118945861361</v>
       </c>
       <c r="X19" t="inlineStr">
         <is>
@@ -2816,63 +2816,63 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.002535909702605</v>
+        <v>0.9972848521456855</v>
       </c>
       <c r="D20" t="n">
-        <v>4.267564403359554e-05</v>
+        <v>4.886401020447739e-05</v>
       </c>
       <c r="E20" t="n">
-        <v>179.4000897181691</v>
+        <v>282.5954338791801</v>
       </c>
       <c r="F20" t="n">
-        <v>1399.254872649988</v>
+        <v>1399.254872650147</v>
       </c>
       <c r="G20" t="n">
-        <v>1219.854782931819</v>
+        <v>1116.659438770967</v>
       </c>
       <c r="H20" t="n">
-        <v>12588.64682794502</v>
+        <v>12588.64683132001</v>
       </c>
       <c r="I20" t="n">
-        <v>2668.562568071502</v>
+        <v>4241.197337490735</v>
       </c>
       <c r="J20" t="n">
-        <v>64.64519477834997</v>
+        <v>64.6451949172981</v>
       </c>
       <c r="K20" t="n">
-        <v>15.68242879445699</v>
+        <v>11.84960753812245</v>
       </c>
       <c r="L20" t="n">
-        <v>4.267564403359554e-05</v>
+        <v>4.886401020447739e-05</v>
       </c>
       <c r="M20" t="n">
-        <v>0.439058941515185</v>
+        <v>0.4390589410827008</v>
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
         <v>0.00655</v>
       </c>
       <c r="P20" t="n">
-        <v>0.5510502550608629</v>
+        <v>0.551050257230309</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.4289518596486359</v>
+        <v>0.4534045207368897</v>
       </c>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="n">
-        <v>0.003963843590413847</v>
+        <v>0.01215643741579669</v>
       </c>
       <c r="T20" t="n">
-        <v>0.4936271891379686</v>
+        <v>0.3002063619988237</v>
       </c>
       <c r="U20" t="n">
-        <v>1.002477158962464</v>
+        <v>0.9972188411292108</v>
       </c>
       <c r="V20" t="n">
-        <v>1.00259466732939</v>
+        <v>0.9973508719019526</v>
       </c>
       <c r="W20" t="n">
-        <v>80.32762357280697</v>
+        <v>76.49480245542055</v>
       </c>
       <c r="X20" t="inlineStr">
         <is>
@@ -2938,63 +2938,63 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.002530497101949</v>
+        <v>0.9972818376306362</v>
       </c>
       <c r="D21" t="n">
-        <v>4.125668840232856e-05</v>
+        <v>4.575113656610273e-05</v>
       </c>
       <c r="E21" t="n">
-        <v>179.4010582882486</v>
+        <v>282.59628808925</v>
       </c>
       <c r="F21" t="n">
-        <v>1399.241745145156</v>
+        <v>1399.241745145151</v>
       </c>
       <c r="G21" t="n">
-        <v>1219.840686856907</v>
+        <v>1116.645457055901</v>
       </c>
       <c r="H21" t="n">
-        <v>11945.31065748219</v>
+        <v>11945.31065045132</v>
       </c>
       <c r="I21" t="n">
-        <v>2560.52119114299</v>
+        <v>4491.164396086388</v>
       </c>
       <c r="J21" t="n">
-        <v>61.85836168721217</v>
+        <v>61.8583615987184</v>
       </c>
       <c r="K21" t="n">
-        <v>13.57048671485295</v>
+        <v>12.69350079877464</v>
       </c>
       <c r="L21" t="n">
-        <v>4.125668840232856e-05</v>
+        <v>4.575113656610273e-05</v>
       </c>
       <c r="M21" t="n">
-        <v>0.4428187160492774</v>
+        <v>0.4428187163957512</v>
       </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
         <v>0.00643</v>
       </c>
       <c r="P21" t="n">
-        <v>0.5322288204111819</v>
+        <v>0.5322288175086354</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.4247978592200549</v>
+        <v>0.4583006832229925</v>
       </c>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="n">
-        <v>0.003665679600189924</v>
+        <v>0.01121680713132682</v>
       </c>
       <c r="T21" t="n">
-        <v>0.4988655005116298</v>
+        <v>0.2705447465282427</v>
       </c>
       <c r="U21" t="n">
-        <v>1.002474083515256</v>
+        <v>0.9972195659657563</v>
       </c>
       <c r="V21" t="n">
-        <v>1.002586917038276</v>
+        <v>0.997344117073146</v>
       </c>
       <c r="W21" t="n">
-        <v>75.42884840206511</v>
+        <v>74.55186239749304</v>
       </c>
       <c r="X21" t="inlineStr">
         <is>
@@ -3060,63 +3060,63 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.00255256035095</v>
+        <v>0.9972854055576105</v>
       </c>
       <c r="D22" t="n">
-        <v>4.159352552264694e-05</v>
+        <v>4.7822662750829e-05</v>
       </c>
       <c r="E22" t="n">
-        <v>179.3971101957727</v>
+        <v>282.5952770618014</v>
       </c>
       <c r="F22" t="n">
-        <v>1399.250988595077</v>
+        <v>1399.250988594828</v>
       </c>
       <c r="G22" t="n">
-        <v>1219.853878399305</v>
+        <v>1116.655711533027</v>
       </c>
       <c r="H22" t="n">
-        <v>12570.1741421898</v>
+        <v>12570.17418707135</v>
       </c>
       <c r="I22" t="n">
-        <v>2687.149111207678</v>
+        <v>4334.56264216619</v>
       </c>
       <c r="J22" t="n">
-        <v>64.63026923690708</v>
+        <v>64.63026964183287</v>
       </c>
       <c r="K22" t="n">
-        <v>14.44898279668858</v>
+        <v>11.78493067850383</v>
       </c>
       <c r="L22" t="n">
-        <v>4.159352552264694e-05</v>
+        <v>4.7822662750829e-05</v>
       </c>
       <c r="M22" t="n">
-        <v>0.4427201391463699</v>
+        <v>0.4427201375812689</v>
       </c>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
         <v>0.00637</v>
       </c>
       <c r="P22" t="n">
-        <v>0.5334384954220086</v>
+        <v>0.5334385110472623</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.4255902033450943</v>
+        <v>0.4545502569420428</v>
       </c>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="n">
-        <v>0.003885992364027438</v>
+        <v>0.01191904744765186</v>
       </c>
       <c r="T22" t="n">
-        <v>0.5051918548641879</v>
+        <v>0.2999380291050648</v>
       </c>
       <c r="U22" t="n">
-        <v>1.002495248482313</v>
+        <v>0.9972208672541161</v>
       </c>
       <c r="V22" t="n">
-        <v>1.002609878772912</v>
+        <v>0.9973499522152466</v>
       </c>
       <c r="W22" t="n">
-        <v>79.07925203359567</v>
+        <v>76.41520032033669</v>
       </c>
       <c r="X22" t="inlineStr">
         <is>
@@ -3182,63 +3182,63 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.002531382817691</v>
+        <v>0.9972741265988673</v>
       </c>
       <c r="D23" t="n">
-        <v>4.210976574108627e-05</v>
+        <v>4.732820636453446e-05</v>
       </c>
       <c r="E23" t="n">
-        <v>179.4008997911239</v>
+        <v>282.5984731544163</v>
       </c>
       <c r="F23" t="n">
-        <v>1399.24558821196</v>
+        <v>1399.245588212064</v>
       </c>
       <c r="G23" t="n">
-        <v>1219.844688420837</v>
+        <v>1116.647115057648</v>
       </c>
       <c r="H23" t="n">
-        <v>12465.43217773761</v>
+        <v>12465.43223888202</v>
       </c>
       <c r="I23" t="n">
-        <v>2630.035150131354</v>
+        <v>4342.401014243318</v>
       </c>
       <c r="J23" t="n">
-        <v>65.05631686536266</v>
+        <v>65.05631766903154</v>
       </c>
       <c r="K23" t="n">
-        <v>14.90075833487614</v>
+        <v>12.76657447945282</v>
       </c>
       <c r="L23" t="n">
-        <v>4.210976574108627e-05</v>
+        <v>4.732820636453445e-05</v>
       </c>
       <c r="M23" t="n">
-        <v>0.4454715042261681</v>
+        <v>0.4454715012013401</v>
       </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
         <v>0.00653</v>
       </c>
       <c r="P23" t="n">
-        <v>0.5392571483156905</v>
+        <v>0.539257172661317</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.4302879095829226</v>
+        <v>0.457010634140955</v>
       </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="n">
-        <v>0.003798686807993864</v>
+        <v>0.01167246693746059</v>
       </c>
       <c r="T23" t="n">
-        <v>0.492868964223494</v>
+        <v>0.2799606137618459</v>
       </c>
       <c r="U23" t="n">
-        <v>1.002473667184415</v>
+        <v>0.997209895253434</v>
       </c>
       <c r="V23" t="n">
-        <v>1.002589105097099</v>
+        <v>0.9973383662192515</v>
       </c>
       <c r="W23" t="n">
-        <v>79.95707520023879</v>
+        <v>77.82289214848436</v>
       </c>
       <c r="X23" t="inlineStr">
         <is>
@@ -3304,63 +3304,63 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.00252669577315</v>
+        <v>0.997270885596346</v>
       </c>
       <c r="D24" t="n">
-        <v>4.087513798401077e-05</v>
+        <v>4.574758196571692e-05</v>
       </c>
       <c r="E24" t="n">
-        <v>179.4017385318894</v>
+        <v>282.599391563223</v>
       </c>
       <c r="F24" t="n">
-        <v>1399.24512779231</v>
+        <v>1399.245127792242</v>
       </c>
       <c r="G24" t="n">
-        <v>1219.843389260421</v>
+        <v>1116.645736229019</v>
       </c>
       <c r="H24" t="n">
-        <v>12301.47506513616</v>
+        <v>12301.47505613598</v>
       </c>
       <c r="I24" t="n">
-        <v>2587.980333606333</v>
+        <v>4460.268201046609</v>
       </c>
       <c r="J24" t="n">
-        <v>62.61583354800056</v>
+        <v>62.61583338903288</v>
       </c>
       <c r="K24" t="n">
-        <v>14.70393355578086</v>
+        <v>13.07598597480066</v>
       </c>
       <c r="L24" t="n">
-        <v>4.087513798401077e-05</v>
+        <v>4.574758196571692e-05</v>
       </c>
       <c r="M24" t="n">
-        <v>0.4421198257773564</v>
+        <v>0.4421198263438217</v>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
         <v>0.0062</v>
       </c>
       <c r="P24" t="n">
-        <v>0.5293258148041663</v>
+        <v>0.5293258107604308</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.4310372621959029</v>
+        <v>0.4541008147507578</v>
       </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="n">
-        <v>0.003915855922790343</v>
+        <v>0.01134457399903894</v>
       </c>
       <c r="T24" t="n">
-        <v>0.4827292573768305</v>
+        <v>0.3044351938707684</v>
       </c>
       <c r="U24" t="n">
-        <v>1.002470169878315</v>
+        <v>0.9972089760268471</v>
       </c>
       <c r="V24" t="n">
-        <v>1.002583228042951</v>
+        <v>0.9973328028533666</v>
       </c>
       <c r="W24" t="n">
-        <v>77.31976710378142</v>
+        <v>75.69181936383353</v>
       </c>
       <c r="X24" t="inlineStr">
         <is>
@@ -3426,63 +3426,63 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.002521115687873</v>
+        <v>0.9972842751195219</v>
       </c>
       <c r="D25" t="n">
-        <v>4.090165276982342e-05</v>
+        <v>4.921111949400546e-05</v>
       </c>
       <c r="E25" t="n">
-        <v>179.402737091405</v>
+        <v>282.5955973881846</v>
       </c>
       <c r="F25" t="n">
-        <v>1399.242967921832</v>
+        <v>1399.242967921819</v>
       </c>
       <c r="G25" t="n">
-        <v>1219.840230830427</v>
+        <v>1116.647370533634</v>
       </c>
       <c r="H25" t="n">
-        <v>12026.79713348537</v>
+        <v>12026.79712582903</v>
       </c>
       <c r="I25" t="n">
-        <v>2613.188345226527</v>
+        <v>4101.153869931458</v>
       </c>
       <c r="J25" t="n">
-        <v>60.97468062506907</v>
+        <v>60.97468052180886</v>
       </c>
       <c r="K25" t="n">
-        <v>14.66050585908414</v>
+        <v>12.94010960149286</v>
       </c>
       <c r="L25" t="n">
-        <v>4.090165276982342e-05</v>
+        <v>4.921111949400547e-05</v>
       </c>
       <c r="M25" t="n">
-        <v>0.4435467175585177</v>
+        <v>0.443546717952081</v>
       </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
         <v>0.00623</v>
       </c>
       <c r="P25" t="n">
-        <v>0.5264437859537708</v>
+        <v>0.5264437827670779</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.4270323033761351</v>
+        <v>0.4497923104267718</v>
       </c>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="n">
-        <v>0.003877036692344795</v>
+        <v>0.0124333204593484</v>
       </c>
       <c r="T25" t="n">
-        <v>0.4896964378983753</v>
+        <v>0.3093050558151199</v>
       </c>
       <c r="U25" t="n">
-        <v>1.002464639699489</v>
+        <v>0.9972184163197253</v>
       </c>
       <c r="V25" t="n">
-        <v>1.002577598040007</v>
+        <v>0.9973501426188528</v>
       </c>
       <c r="W25" t="n">
-        <v>75.63518648415321</v>
+        <v>73.91479012330173</v>
       </c>
       <c r="X25" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
New pickles, photo thing etc., remove scipy gaussian import
</commit_message>
<xml_diff>
--- a/docs/UCB_Densimeter_fitting/Full_Datasets/Used_in_Calibration_2023/UCB_6-8-23/PseudoVoigt.xlsx
+++ b/docs/UCB_Densimeter_fitting/Full_Datasets/Used_in_Calibration_2023/UCB_6-8-23/PseudoVoigt.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AL25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,65 +546,75 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
+          <t>error_pk1_amplitude</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>error_pk2_amplitude</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
           <t>name_for_matching</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>filename_y</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Day</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>power (mW)</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Int_time (s)</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>accumulations</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Mag (X)</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>duration</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>24hr_time</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>sec since midnight</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Spectral Center</t>
         </is>
@@ -616,119 +626,125 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ne1.txt</t>
+          <t>01 Ne1.txt</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9973520204120639</v>
+        <v>0.9972143774491398</v>
       </c>
       <c r="D2" t="n">
-        <v>4.969691439133369e-05</v>
+        <v>2.682516147009868e-05</v>
       </c>
       <c r="E2" t="n">
-        <v>282.5764020378726</v>
+        <v>228.0925386851286</v>
       </c>
       <c r="F2" t="n">
-        <v>1399.18178038813</v>
+        <v>1447.876817123708</v>
       </c>
       <c r="G2" t="n">
-        <v>1116.605378350257</v>
+        <v>1219.78427843858</v>
       </c>
       <c r="H2" t="n">
-        <v>12400.74198105815</v>
+        <v>44806.50030668431</v>
       </c>
       <c r="I2" t="n">
-        <v>4087.888743058904</v>
+        <v>2798.27364967129</v>
       </c>
       <c r="J2" t="n">
-        <v>61.88927284178892</v>
+        <v>143.0078196585313</v>
       </c>
       <c r="K2" t="n">
-        <v>11.27181845584035</v>
+        <v>26.41093936876095</v>
       </c>
       <c r="L2" t="n">
-        <v>4.96969143913337e-05</v>
+        <v>2.682516147009868e-05</v>
       </c>
       <c r="M2" t="n">
-        <v>0.441596158182409</v>
+        <v>0.4800000000221231</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
-        <v>0.0063</v>
+        <v>0.002808196974901238</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4988515847758431</v>
+        <v>0.1436456758918967</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4487858101455117</v>
+        <v>0.4800000000018776</v>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
-        <v>0.01255072792365499</v>
+        <v>0.005436131935884456</v>
       </c>
       <c r="T2" t="n">
-        <v>0.2923131503078331</v>
+        <v>0.4484041357741383</v>
       </c>
       <c r="U2" t="n">
-        <v>0.997285491298794</v>
+        <v>0.9971783347700497</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9974185584022668</v>
+        <v>0.9972504227338254</v>
       </c>
       <c r="W2" t="n">
-        <v>73.16109129762927</v>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>Ne1</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>Ne1.txt</t>
-        </is>
+        <v>169.4187590272923</v>
+      </c>
+      <c r="X2" t="n">
+        <v>54.78707588155321</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>469.3378582746195</v>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
+          <t>01 Ne1</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>01 Ne1.txt</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB2" t="n">
+      <c r="AD2" t="n">
         <v>8</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AE2" t="n">
         <v>34.43</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AF2" t="n">
         <v>45</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AG2" t="n">
         <v>3</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AH2" t="n">
         <v>5</v>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>['0h', '2m', '19s']</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t xml:space="preserve">12:01:31 PM
 </t>
         </is>
       </c>
-      <c r="AI2" t="n">
+      <c r="AK2" t="n">
         <v>43291</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AL2" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -738,119 +754,125 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ne2.txt</t>
+          <t>02 Ne2.txt</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9973638843918695</v>
+        <v>0.9972199579681641</v>
       </c>
       <c r="D3" t="n">
-        <v>4.943461771075839e-05</v>
+        <v>2.634040389104475e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>282.5730406962603</v>
+        <v>228.0912622618669</v>
       </c>
       <c r="F3" t="n">
-        <v>1399.186713091324</v>
+        <v>1447.883142584404</v>
       </c>
       <c r="G3" t="n">
-        <v>1116.613672395064</v>
+        <v>1219.791880322537</v>
       </c>
       <c r="H3" t="n">
-        <v>11791.86922669792</v>
+        <v>44012.91735041975</v>
       </c>
       <c r="I3" t="n">
-        <v>4136.27448377201</v>
+        <v>2731.65765750011</v>
       </c>
       <c r="J3" t="n">
-        <v>60.55961346136612</v>
+        <v>138.6602489538527</v>
       </c>
       <c r="K3" t="n">
-        <v>9.722830923066146</v>
+        <v>24.99988068202704</v>
       </c>
       <c r="L3" t="n">
-        <v>4.943461771075839e-05</v>
+        <v>2.634040389104475e-05</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4442725144561843</v>
+        <v>0.4800000001037292</v>
       </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="n">
-        <v>0.00643</v>
+        <v>0.002697250754992297</v>
       </c>
       <c r="P3" t="n">
-        <v>0.499952696862576</v>
+        <v>0.1353017274974086</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.4450867738716393</v>
+        <v>0.4800000000925684</v>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
-        <v>0.01240100780574889</v>
+        <v>0.005368528130172176</v>
       </c>
       <c r="T3" t="n">
-        <v>0.3133569696324933</v>
+        <v>0.437836273770765</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9972974232902859</v>
+        <v>0.9971846954544596</v>
       </c>
       <c r="V3" t="n">
-        <v>0.9974303543521391</v>
+        <v>0.9972552229758676</v>
       </c>
       <c r="W3" t="n">
-        <v>70.28244438443227</v>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>Ne2</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>Ne2.txt</t>
-        </is>
+        <v>163.6601296358798</v>
+      </c>
+      <c r="X3" t="n">
+        <v>65.10880719376138</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>524.7744916909668</v>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
+          <t>02 Ne2</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>02 Ne2.txt</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB3" t="n">
+      <c r="AD3" t="n">
         <v>8</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AE3" t="n">
         <v>34.438</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AF3" t="n">
         <v>45</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AG3" t="n">
         <v>3</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AH3" t="n">
         <v>5</v>
       </c>
-      <c r="AG3" t="inlineStr">
+      <c r="AI3" t="inlineStr">
         <is>
           <t>['0h', '2m', '16s']</t>
         </is>
       </c>
-      <c r="AH3" t="inlineStr">
+      <c r="AJ3" t="inlineStr">
         <is>
           <t xml:space="preserve">12:05:23 PM
 </t>
         </is>
       </c>
-      <c r="AI3" t="n">
+      <c r="AK3" t="n">
         <v>43523</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AL3" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -860,119 +882,125 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ne3.txt</t>
+          <t>03 Ne3.txt</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9973461595108428</v>
+        <v>0.9971901627628562</v>
       </c>
       <c r="D4" t="n">
-        <v>4.96312655553865e-05</v>
+        <v>2.704400528800308e-05</v>
       </c>
       <c r="E4" t="n">
-        <v>282.5780625971117</v>
+        <v>228.0980774373888</v>
       </c>
       <c r="F4" t="n">
-        <v>1399.192097159655</v>
+        <v>1447.885614491374</v>
       </c>
       <c r="G4" t="n">
-        <v>1116.614034562543</v>
+        <v>1219.787537053985</v>
       </c>
       <c r="H4" t="n">
-        <v>12012.65727920115</v>
+        <v>44181.57986614105</v>
       </c>
       <c r="I4" t="n">
-        <v>4051.373774169645</v>
+        <v>2762.122391261602</v>
       </c>
       <c r="J4" t="n">
-        <v>61.96330442919957</v>
+        <v>137.7797413166381</v>
       </c>
       <c r="K4" t="n">
-        <v>11.30907354150381</v>
+        <v>26.60942789804926</v>
       </c>
       <c r="L4" t="n">
-        <v>4.963126555538649e-05</v>
+        <v>2.704400528800308e-05</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4430201050851046</v>
+        <v>0.4800000000000086</v>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>0.00644</v>
+        <v>0.002652545083762245</v>
       </c>
       <c r="P4" t="n">
-        <v>0.4996338360641645</v>
+        <v>0.131012907930964</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.4502818219734405</v>
+        <v>0.4800000000005097</v>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
-        <v>0.01245868382478346</v>
+        <v>0.00556926267680386</v>
       </c>
       <c r="T4" t="n">
-        <v>0.2739466231992534</v>
+        <v>0.4525488212712385</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9972794619439361</v>
+        <v>0.997154220284082</v>
       </c>
       <c r="V4" t="n">
-        <v>0.9974128659997481</v>
+        <v>0.9972261078328211</v>
       </c>
       <c r="W4" t="n">
-        <v>73.27237797070339</v>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Ne3</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Ne3.txt</t>
-        </is>
+        <v>164.3891692146873</v>
+      </c>
+      <c r="X4" t="n">
+        <v>60.9285287815864</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>520.8981018444676</v>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
+          <t>03 Ne3</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>03 Ne3.txt</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AC4" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB4" t="n">
+      <c r="AD4" t="n">
         <v>8</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AE4" t="n">
         <v>34.495</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AF4" t="n">
         <v>45</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AG4" t="n">
         <v>3</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AH4" t="n">
         <v>5</v>
       </c>
-      <c r="AG4" t="inlineStr">
+      <c r="AI4" t="inlineStr">
         <is>
           <t>['0h', '2m', '16s']</t>
         </is>
       </c>
-      <c r="AH4" t="inlineStr">
+      <c r="AJ4" t="inlineStr">
         <is>
           <t xml:space="preserve">12:09:28 PM
 </t>
         </is>
       </c>
-      <c r="AI4" t="n">
+      <c r="AK4" t="n">
         <v>43768</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AL4" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -982,119 +1010,125 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ne4.txt</t>
+          <t>04 Ne4.txt</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9973488492797445</v>
+        <v>0.9971995388501415</v>
       </c>
       <c r="D5" t="n">
-        <v>4.859929415464578e-05</v>
+        <v>2.60988650123876e-05</v>
       </c>
       <c r="E5" t="n">
-        <v>282.5773005070109</v>
+        <v>228.0959327638302</v>
       </c>
       <c r="F5" t="n">
-        <v>1399.193628174454</v>
+        <v>1447.888479637278</v>
       </c>
       <c r="G5" t="n">
-        <v>1116.616327667443</v>
+        <v>1219.792546873448</v>
       </c>
       <c r="H5" t="n">
-        <v>11802.74976107666</v>
+        <v>43936.91625990171</v>
       </c>
       <c r="I5" t="n">
-        <v>4153.10817521906</v>
+        <v>2695.506548550507</v>
       </c>
       <c r="J5" t="n">
-        <v>60.26989246331013</v>
+        <v>132.8669512652635</v>
       </c>
       <c r="K5" t="n">
-        <v>11.2603338829141</v>
+        <v>25.2596040338646</v>
       </c>
       <c r="L5" t="n">
-        <v>4.859929415464577e-05</v>
+        <v>2.60988650123876e-05</v>
       </c>
       <c r="M5" t="n">
-        <v>0.4415880924233843</v>
+        <v>0.4800000000226374</v>
       </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.00637</v>
+        <v>0.002628962161845395</v>
       </c>
       <c r="P5" t="n">
-        <v>0.5097294661577725</v>
+        <v>0.1375145322347754</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.4452370532199176</v>
+        <v>0.4800000000000974</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="n">
-        <v>0.01216634555421203</v>
+        <v>0.005341095602625673</v>
       </c>
       <c r="T5" t="n">
-        <v>0.2835597870511327</v>
+        <v>0.4372254098172941</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9972834300466999</v>
+        <v>0.9971646962287344</v>
       </c>
       <c r="V5" t="n">
-        <v>0.9974142770960198</v>
+        <v>0.9972343839065539</v>
       </c>
       <c r="W5" t="n">
-        <v>71.53022634622423</v>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>Ne4</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>Ne4.txt</t>
-        </is>
+        <v>158.1265552991281</v>
+      </c>
+      <c r="X5" t="n">
+        <v>55.96523668747627</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>514.271782855795</v>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
+          <t>04 Ne4</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>04 Ne4.txt</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA5" t="inlineStr">
+      <c r="AC5" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB5" t="n">
+      <c r="AD5" t="n">
         <v>8</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AE5" t="n">
         <v>34.506</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AF5" t="n">
         <v>45</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AG5" t="n">
         <v>3</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AH5" t="n">
         <v>5</v>
       </c>
-      <c r="AG5" t="inlineStr">
+      <c r="AI5" t="inlineStr">
         <is>
           <t>['0h', '2m', '16s']</t>
         </is>
       </c>
-      <c r="AH5" t="inlineStr">
+      <c r="AJ5" t="inlineStr">
         <is>
           <t xml:space="preserve">12:12:54 PM
 </t>
         </is>
       </c>
-      <c r="AI5" t="n">
+      <c r="AK5" t="n">
         <v>43974</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AL5" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -1104,119 +1138,125 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ne5.txt</t>
+          <t>05 Ne5.txt</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9973343751379473</v>
+        <v>0.9971928771900901</v>
       </c>
       <c r="D6" t="n">
-        <v>4.788973473534765e-05</v>
+        <v>2.588166701939276e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>282.5814015026431</v>
+        <v>228.0974565388169</v>
       </c>
       <c r="F6" t="n">
-        <v>1399.204967005978</v>
+        <v>1447.89625666499</v>
       </c>
       <c r="G6" t="n">
-        <v>1116.623565503335</v>
+        <v>1219.798800126174</v>
       </c>
       <c r="H6" t="n">
-        <v>11812.22228973141</v>
+        <v>46430.77525819019</v>
       </c>
       <c r="I6" t="n">
-        <v>4285.193056264594</v>
+        <v>2735.313630466107</v>
       </c>
       <c r="J6" t="n">
-        <v>61.58716265880887</v>
+        <v>136.2192152226762</v>
       </c>
       <c r="K6" t="n">
-        <v>12.04992137715447</v>
+        <v>24.73656042872835</v>
       </c>
       <c r="L6" t="n">
-        <v>4.788973473534764e-05</v>
+        <v>2.588166701939276e-05</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4425753614292666</v>
+        <v>0.4800000000005237</v>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.00627</v>
+        <v>0.002522254999562538</v>
       </c>
       <c r="P6" t="n">
-        <v>0.5108143615070191</v>
+        <v>0.1383603303540706</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.4517114362258256</v>
+        <v>0.480000000000098</v>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="n">
-        <v>0.01199259680598165</v>
+        <v>0.005337606467283165</v>
       </c>
       <c r="T6" t="n">
-        <v>0.2710449352280883</v>
+        <v>0.4285628384459734</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9972699238385019</v>
+        <v>0.9971585167552079</v>
       </c>
       <c r="V6" t="n">
-        <v>0.9973988347686146</v>
+        <v>0.9972272399930614</v>
       </c>
       <c r="W6" t="n">
-        <v>73.63708403596334</v>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>Ne5</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>Ne5.txt</t>
-        </is>
+        <v>160.9557756514046</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1.056773486794315</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>526.7731562578142</v>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
+          <t>05 Ne5</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>05 Ne5.txt</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
+      <c r="AC6" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB6" t="n">
+      <c r="AD6" t="n">
         <v>8</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AE6" t="n">
         <v>34.477</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AF6" t="n">
         <v>45</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AG6" t="n">
         <v>3</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AH6" t="n">
         <v>5</v>
       </c>
-      <c r="AG6" t="inlineStr">
+      <c r="AI6" t="inlineStr">
         <is>
           <t>['0h', '2m', '16s']</t>
         </is>
       </c>
-      <c r="AH6" t="inlineStr">
+      <c r="AJ6" t="inlineStr">
         <is>
           <t xml:space="preserve">12:23:40 PM
 </t>
         </is>
       </c>
-      <c r="AI6" t="n">
+      <c r="AK6" t="n">
         <v>44620</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="AL6" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -1226,119 +1266,125 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ne6.txt</t>
+          <t>09 Ne6.txt</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9973401245191023</v>
+        <v>0.9971730014471977</v>
       </c>
       <c r="D7" t="n">
-        <v>4.737792921001566e-05</v>
+        <v>2.727925531463307e-05</v>
       </c>
       <c r="E7" t="n">
-        <v>282.5797725015184</v>
+        <v>228.1020029980511</v>
       </c>
       <c r="F7" t="n">
-        <v>1399.205444926253</v>
+        <v>1447.901312232349</v>
       </c>
       <c r="G7" t="n">
-        <v>1116.625672424734</v>
+        <v>1219.799309234298</v>
       </c>
       <c r="H7" t="n">
-        <v>12041.86649462387</v>
+        <v>46353.99943016599</v>
       </c>
       <c r="I7" t="n">
-        <v>4318.870362328328</v>
+        <v>2717.034879582092</v>
       </c>
       <c r="J7" t="n">
-        <v>62.69997228707534</v>
+        <v>133.8804091261914</v>
       </c>
       <c r="K7" t="n">
-        <v>13.2806800270088</v>
+        <v>26.93730751205176</v>
       </c>
       <c r="L7" t="n">
-        <v>4.737792921001566e-05</v>
+        <v>2.727925531463307e-05</v>
       </c>
       <c r="M7" t="n">
-        <v>0.4434865937295057</v>
+        <v>0.4800000000033304</v>
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>0.00643</v>
+        <v>0.002510527255658025</v>
       </c>
       <c r="P7" t="n">
-        <v>0.5092522692140466</v>
+        <v>0.1415887124941835</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.4462671280774959</v>
+        <v>0.4800000000492055</v>
       </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="n">
-        <v>0.0117428631262967</v>
+        <v>0.005693520129726435</v>
       </c>
       <c r="T7" t="n">
-        <v>0.3006303649529763</v>
+        <v>0.4326138642259063</v>
       </c>
       <c r="U7" t="n">
-        <v>0.9972759891427825</v>
+        <v>0.9971371378413503</v>
       </c>
       <c r="V7" t="n">
-        <v>0.9974042681451164</v>
+        <v>0.9972088676329199</v>
       </c>
       <c r="W7" t="n">
-        <v>75.98065231408414</v>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>Ne6</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>Ne6.txt</t>
-        </is>
+        <v>160.8177166382432</v>
+      </c>
+      <c r="X7" t="n">
+        <v>31.06864362620978</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>525.8482200458972</v>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
+          <t>09 Ne6</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>09 Ne6.txt</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA7" t="inlineStr">
+      <c r="AC7" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB7" t="n">
+      <c r="AD7" t="n">
         <v>8</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AE7" t="n">
         <v>34.519</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AF7" t="n">
         <v>45</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AG7" t="n">
         <v>3</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AH7" t="n">
         <v>5</v>
       </c>
-      <c r="AG7" t="inlineStr">
+      <c r="AI7" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH7" t="inlineStr">
+      <c r="AJ7" t="inlineStr">
         <is>
           <t xml:space="preserve">12:35:21 PM
 </t>
         </is>
       </c>
-      <c r="AI7" t="n">
+      <c r="AK7" t="n">
         <v>45321</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AL7" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -1348,119 +1394,125 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ne7.txt</t>
+          <t>13 Ne7.txt</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9973301074586244</v>
+        <v>0.9971868094613271</v>
       </c>
       <c r="D8" t="n">
-        <v>4.689403194396309e-05</v>
+        <v>2.345989063731376e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>282.5826106978686</v>
+        <v>228.0988444768489</v>
       </c>
       <c r="F8" t="n">
-        <v>1399.211512469338</v>
+        <v>1447.905849368918</v>
       </c>
       <c r="G8" t="n">
-        <v>1116.628901771469</v>
+        <v>1219.807004892069</v>
       </c>
       <c r="H8" t="n">
-        <v>12120.82152595241</v>
+        <v>46524.79671596777</v>
       </c>
       <c r="I8" t="n">
-        <v>4372.695117223288</v>
+        <v>2585.021703037155</v>
       </c>
       <c r="J8" t="n">
-        <v>61.40430872492011</v>
+        <v>131.7626195819309</v>
       </c>
       <c r="K8" t="n">
-        <v>11.96833152311517</v>
+        <v>22.55756759687529</v>
       </c>
       <c r="L8" t="n">
-        <v>4.689403194396309e-05</v>
+        <v>2.345989063731376e-05</v>
       </c>
       <c r="M8" t="n">
-        <v>0.4464873298104064</v>
+        <v>0.4800000000045936</v>
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>0.00624</v>
+        <v>0.002441992981560117</v>
       </c>
       <c r="P8" t="n">
-        <v>0.5025513047344334</v>
+        <v>0.1438286911871042</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4519614006846209</v>
+        <v>0.4800000000032862</v>
       </c>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
-        <v>0.01169029547740073</v>
+        <v>0.004761484314533911</v>
       </c>
       <c r="T8" t="n">
-        <v>0.2984159598983991</v>
+        <v>0.4000694924577077</v>
       </c>
       <c r="U8" t="n">
-        <v>0.9972668293649155</v>
+        <v>0.9971553187901837</v>
       </c>
       <c r="V8" t="n">
-        <v>0.9973933935830249</v>
+        <v>0.9972183021215161</v>
       </c>
       <c r="W8" t="n">
-        <v>73.37264024803527</v>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>Ne7</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>Ne7.txt</t>
-        </is>
+        <v>154.3201871788062</v>
+      </c>
+      <c r="X8" t="n">
+        <v>31.44445600096513</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>515.2090492039353</v>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
+          <t>13 Ne7</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>13 Ne7.txt</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA8" t="inlineStr">
+      <c r="AC8" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB8" t="n">
+      <c r="AD8" t="n">
         <v>8</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AE8" t="n">
         <v>34.446</v>
       </c>
-      <c r="AD8" t="n">
+      <c r="AF8" t="n">
         <v>45</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AG8" t="n">
         <v>3</v>
       </c>
-      <c r="AF8" t="n">
+      <c r="AH8" t="n">
         <v>5</v>
       </c>
-      <c r="AG8" t="inlineStr">
+      <c r="AI8" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH8" t="inlineStr">
+      <c r="AJ8" t="inlineStr">
         <is>
           <t xml:space="preserve">12:56:23 PM
 </t>
         </is>
       </c>
-      <c r="AI8" t="n">
+      <c r="AK8" t="n">
         <v>46583</v>
       </c>
-      <c r="AJ8" t="n">
+      <c r="AL8" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -1470,119 +1522,125 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ne8.txt</t>
+          <t>17 Ne8.txt</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.99730004789635</v>
+        <v>0.9971583617566661</v>
       </c>
       <c r="D9" t="n">
-        <v>4.672392926131259e-05</v>
+        <v>2.49927084431231e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>282.5911280037706</v>
+        <v>228.1053518570304</v>
       </c>
       <c r="F9" t="n">
-        <v>1399.224054871444</v>
+        <v>1447.921030436202</v>
       </c>
       <c r="G9" t="n">
-        <v>1116.632926867674</v>
+        <v>1219.815678579172</v>
       </c>
       <c r="H9" t="n">
-        <v>12185.16235351838</v>
+        <v>47483.29048058408</v>
       </c>
       <c r="I9" t="n">
-        <v>4360.286310568194</v>
+        <v>2625.234955325358</v>
       </c>
       <c r="J9" t="n">
-        <v>62.52285233938186</v>
+        <v>126.6362148456891</v>
       </c>
       <c r="K9" t="n">
-        <v>12.58930296860675</v>
+        <v>25.16965710478189</v>
       </c>
       <c r="L9" t="n">
-        <v>4.672392926131259e-05</v>
+        <v>2.49927084431231e-05</v>
       </c>
       <c r="M9" t="n">
-        <v>0.4469409692891353</v>
+        <v>0.4800000000016729</v>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>0.00639</v>
+        <v>0.002328302689409791</v>
       </c>
       <c r="P9" t="n">
-        <v>0.509974553198882</v>
+        <v>0.1505371515656325</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.4519578932635154</v>
+        <v>0.4800000000507227</v>
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="n">
-        <v>0.01155453963122544</v>
+        <v>0.005203851634687404</v>
       </c>
       <c r="T9" t="n">
-        <v>0.3004509863364854</v>
+        <v>0.3893180122709377</v>
       </c>
       <c r="U9" t="n">
-        <v>0.9972367233538193</v>
+        <v>0.9971254361694122</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9973633804816096</v>
+        <v>0.9971912895184311</v>
       </c>
       <c r="W9" t="n">
-        <v>75.11215530798862</v>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>Ne8</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>Ne8.txt</t>
-        </is>
+        <v>151.805871950471</v>
+      </c>
+      <c r="X9" t="n">
+        <v>10.89691722552792</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>504.4754996423543</v>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
+          <t>17 Ne8</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>17 Ne8.txt</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA9" t="inlineStr">
+      <c r="AC9" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB9" t="n">
+      <c r="AD9" t="n">
         <v>8</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AE9" t="n">
         <v>34.314</v>
       </c>
-      <c r="AD9" t="n">
+      <c r="AF9" t="n">
         <v>45</v>
       </c>
-      <c r="AE9" t="n">
+      <c r="AG9" t="n">
         <v>3</v>
       </c>
-      <c r="AF9" t="n">
+      <c r="AH9" t="n">
         <v>5</v>
       </c>
-      <c r="AG9" t="inlineStr">
+      <c r="AI9" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH9" t="inlineStr">
+      <c r="AJ9" t="inlineStr">
         <is>
           <t xml:space="preserve">1:33:05 PM
 </t>
         </is>
       </c>
-      <c r="AI9" t="n">
+      <c r="AK9" t="n">
         <v>48785</v>
       </c>
-      <c r="AJ9" t="n">
+      <c r="AL9" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -1592,119 +1650,125 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ne9.txt</t>
+          <t>19 Ne9.txt</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9972957773588904</v>
+        <v>0.9971533955178812</v>
       </c>
       <c r="D10" t="n">
-        <v>4.748776120982345e-05</v>
+        <v>2.298664170988816e-05</v>
       </c>
       <c r="E10" t="n">
-        <v>282.5923380921167</v>
+        <v>228.1064879165881</v>
       </c>
       <c r="F10" t="n">
-        <v>1399.223622310493</v>
+        <v>1447.922329000168</v>
       </c>
       <c r="G10" t="n">
-        <v>1116.631284218376</v>
+        <v>1219.81584108358</v>
       </c>
       <c r="H10" t="n">
-        <v>11912.79432230535</v>
+        <v>45852.12546633379</v>
       </c>
       <c r="I10" t="n">
-        <v>4408.839042955176</v>
+        <v>2605.737402188555</v>
       </c>
       <c r="J10" t="n">
-        <v>62.86195344495396</v>
+        <v>118.6402647197864</v>
       </c>
       <c r="K10" t="n">
-        <v>12.57959801904356</v>
+        <v>22.65510858172361</v>
       </c>
       <c r="L10" t="n">
-        <v>4.748776120982345e-05</v>
+        <v>2.298664170988817e-05</v>
       </c>
       <c r="M10" t="n">
-        <v>0.4437729929158654</v>
+        <v>0.4800000000226828</v>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>0.00645</v>
+        <v>0.002277599138413328</v>
       </c>
       <c r="P10" t="n">
-        <v>0.5234299559448446</v>
+        <v>0.1538410743300294</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.453902124791588</v>
+        <v>0.4800000000131692</v>
       </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="n">
-        <v>0.01176797533252214</v>
+        <v>0.0047229024810993</v>
       </c>
       <c r="T10" t="n">
-        <v>0.2970989859129086</v>
+        <v>0.3871693013743697</v>
       </c>
       <c r="U10" t="n">
-        <v>0.9972314885010216</v>
+        <v>0.9971227941974223</v>
       </c>
       <c r="V10" t="n">
-        <v>0.9973600745063566</v>
+        <v>0.9971839987166835</v>
       </c>
       <c r="W10" t="n">
-        <v>75.44155146399751</v>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>Ne9</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>Ne9.txt</t>
-        </is>
+        <v>141.29537330151</v>
+      </c>
+      <c r="X10" t="n">
+        <v>33.81456283436207</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>476.0884251474598</v>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
+          <t>19 Ne9</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>19 Ne9.txt</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA10" t="inlineStr">
+      <c r="AC10" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB10" t="n">
+      <c r="AD10" t="n">
         <v>8</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AE10" t="n">
         <v>34.255</v>
       </c>
-      <c r="AD10" t="n">
+      <c r="AF10" t="n">
         <v>45</v>
       </c>
-      <c r="AE10" t="n">
+      <c r="AG10" t="n">
         <v>3</v>
       </c>
-      <c r="AF10" t="n">
+      <c r="AH10" t="n">
         <v>5</v>
       </c>
-      <c r="AG10" t="inlineStr">
+      <c r="AI10" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH10" t="inlineStr">
+      <c r="AJ10" t="inlineStr">
         <is>
           <t xml:space="preserve">1:48:33 PM
 </t>
         </is>
       </c>
-      <c r="AI10" t="n">
+      <c r="AK10" t="n">
         <v>49713</v>
       </c>
-      <c r="AJ10" t="n">
+      <c r="AL10" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -1714,119 +1778,125 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ne10.txt</t>
+          <t>21 Ne10.txt</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9973067865889192</v>
+        <v>0.9971577899284343</v>
       </c>
       <c r="D11" t="n">
-        <v>4.70067368953022e-05</v>
+        <v>2.351346889128004e-05</v>
       </c>
       <c r="E11" t="n">
-        <v>282.5892185665141</v>
+        <v>228.1054826658967</v>
       </c>
       <c r="F11" t="n">
-        <v>1399.223440668404</v>
+        <v>1447.918684581068</v>
       </c>
       <c r="G11" t="n">
-        <v>1116.634222101889</v>
+        <v>1219.813201915171</v>
       </c>
       <c r="H11" t="n">
-        <v>12086.62801199748</v>
+        <v>47797.55660581751</v>
       </c>
       <c r="I11" t="n">
-        <v>4432.393918631524</v>
+        <v>2756.841813922902</v>
       </c>
       <c r="J11" t="n">
-        <v>66.20818617751884</v>
+        <v>128.2731253842865</v>
       </c>
       <c r="K11" t="n">
-        <v>10.70067323119609</v>
+        <v>23.91256707317645</v>
       </c>
       <c r="L11" t="n">
-        <v>4.70067368953022e-05</v>
+        <v>2.351346889128004e-05</v>
       </c>
       <c r="M11" t="n">
-        <v>0.44566118618364</v>
+        <v>0.4800000000011612</v>
       </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>0.00667</v>
+        <v>0.002316671089736704</v>
       </c>
       <c r="P11" t="n">
-        <v>0.5253006050868078</v>
+        <v>0.1497506018333707</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.4528557008495996</v>
+        <v>0.4800000000051379</v>
       </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
-        <v>0.01148760421047739</v>
+        <v>0.004837428678706172</v>
       </c>
       <c r="T11" t="n">
-        <v>0.3078645875735523</v>
+        <v>0.3924268454276298</v>
       </c>
       <c r="U11" t="n">
-        <v>0.9972427093445363</v>
+        <v>0.9971265169292036</v>
       </c>
       <c r="V11" t="n">
-        <v>0.9973708720683228</v>
+        <v>0.9971890648893643</v>
       </c>
       <c r="W11" t="n">
-        <v>76.90885940871493</v>
-      </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>Ne10</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>Ne10.txt</t>
-        </is>
+        <v>152.1856924574629</v>
+      </c>
+      <c r="X11" t="n">
+        <v>39.45033794468331</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>505.0803258693596</v>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
+          <t>21 Ne10</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>21 Ne10.txt</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA11" t="inlineStr">
+      <c r="AC11" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB11" t="n">
+      <c r="AD11" t="n">
         <v>8</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AE11" t="n">
         <v>34.296</v>
       </c>
-      <c r="AD11" t="n">
+      <c r="AF11" t="n">
         <v>45</v>
       </c>
-      <c r="AE11" t="n">
+      <c r="AG11" t="n">
         <v>3</v>
       </c>
-      <c r="AF11" t="n">
+      <c r="AH11" t="n">
         <v>5</v>
       </c>
-      <c r="AG11" t="inlineStr">
+      <c r="AI11" t="inlineStr">
         <is>
           <t>['0h', '2m', '16s']</t>
         </is>
       </c>
-      <c r="AH11" t="inlineStr">
+      <c r="AJ11" t="inlineStr">
         <is>
           <t xml:space="preserve">2:02:15 PM
 </t>
         </is>
       </c>
-      <c r="AI11" t="n">
+      <c r="AK11" t="n">
         <v>50535</v>
       </c>
-      <c r="AJ11" t="n">
+      <c r="AL11" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -1836,119 +1906,125 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ne11.txt</t>
+          <t>23 Ne11.txt</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9972971197581304</v>
+        <v>0.9972504673638868</v>
       </c>
       <c r="D12" t="n">
-        <v>4.625640437674619e-05</v>
+        <v>6.635009756572793e-05</v>
       </c>
       <c r="E12" t="n">
-        <v>282.5919577122556</v>
+        <v>228.0842841487358</v>
       </c>
       <c r="F12" t="n">
-        <v>1399.217582650051</v>
+        <v>1447.911921367033</v>
       </c>
       <c r="G12" t="n">
-        <v>1116.625624937795</v>
+        <v>1219.827637218297</v>
       </c>
       <c r="H12" t="n">
-        <v>11610.7553457122</v>
+        <v>45188.49329109385</v>
       </c>
       <c r="I12" t="n">
-        <v>4462.216248167377</v>
+        <v>3410.540595885655</v>
       </c>
       <c r="J12" t="n">
-        <v>59.63211371518476</v>
+        <v>118.7793795931526</v>
       </c>
       <c r="K12" t="n">
-        <v>11.82165249163777</v>
+        <v>45.27541202252096</v>
       </c>
       <c r="L12" t="n">
-        <v>4.625640437674619e-05</v>
+        <v>6.635009756572793e-05</v>
       </c>
       <c r="M12" t="n">
-        <v>0.4451437488737612</v>
+        <v>0.4800000000051225</v>
       </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>0.00635</v>
+        <v>0.002330047125793201</v>
       </c>
       <c r="P12" t="n">
-        <v>0.5159097037007931</v>
+        <v>0.162854574751253</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.4555767296923172</v>
+        <v>0.4800000005651317</v>
       </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="n">
-        <v>0.01142569576695691</v>
+        <v>0.0149529634192175</v>
       </c>
       <c r="T12" t="n">
-        <v>0.3034412112657271</v>
+        <v>0.9402640959103072</v>
       </c>
       <c r="U12" t="n">
-        <v>0.9972343913801073</v>
+        <v>0.9971749067679726</v>
       </c>
       <c r="V12" t="n">
-        <v>0.9973598560281737</v>
+        <v>0.9973260394118265</v>
       </c>
       <c r="W12" t="n">
-        <v>71.45376620682252</v>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>Ne11</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>Ne11.txt</t>
-        </is>
+        <v>164.0547916156736</v>
+      </c>
+      <c r="X12" t="n">
+        <v>98.82985745460311</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>476.4380474835906</v>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
+          <t>23 Ne11</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>23 Ne11.txt</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA12" t="inlineStr">
+      <c r="AC12" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB12" t="n">
+      <c r="AD12" t="n">
         <v>8</v>
       </c>
-      <c r="AC12" t="n">
+      <c r="AE12" t="n">
         <v>34.363</v>
       </c>
-      <c r="AD12" t="n">
+      <c r="AF12" t="n">
         <v>45</v>
       </c>
-      <c r="AE12" t="n">
+      <c r="AG12" t="n">
         <v>3</v>
       </c>
-      <c r="AF12" t="n">
+      <c r="AH12" t="n">
         <v>5</v>
       </c>
-      <c r="AG12" t="inlineStr">
+      <c r="AI12" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH12" t="inlineStr">
+      <c r="AJ12" t="inlineStr">
         <is>
           <t xml:space="preserve">2:11:18 PM
 </t>
         </is>
       </c>
-      <c r="AI12" t="n">
+      <c r="AK12" t="n">
         <v>51078</v>
       </c>
-      <c r="AJ12" t="n">
+      <c r="AL12" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -1958,119 +2034,125 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ne12.txt</t>
+          <t>26 Ne12.txt</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.9972912268873316</v>
+        <v>0.9971491822321417</v>
       </c>
       <c r="D13" t="n">
-        <v>4.763998142828519e-05</v>
+        <v>2.360290504895274e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>282.5936275132633</v>
+        <v>228.1074517420916</v>
       </c>
       <c r="F13" t="n">
-        <v>1399.220686633032</v>
+        <v>1447.918056824597</v>
       </c>
       <c r="G13" t="n">
-        <v>1116.627059119768</v>
+        <v>1219.810605082505</v>
       </c>
       <c r="H13" t="n">
-        <v>11941.72559917746</v>
+        <v>44968.96644138331</v>
       </c>
       <c r="I13" t="n">
-        <v>4324.5987828516</v>
+        <v>2643.513483557155</v>
       </c>
       <c r="J13" t="n">
-        <v>60.91988661065819</v>
+        <v>117.6885276187735</v>
       </c>
       <c r="K13" t="n">
-        <v>11.8770840426474</v>
+        <v>24.79090810623094</v>
       </c>
       <c r="L13" t="n">
-        <v>4.763998142828519e-05</v>
+        <v>2.360290504895274e-05</v>
       </c>
       <c r="M13" t="n">
-        <v>0.4446520507981164</v>
+        <v>0.4800000000037615</v>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>0.00621</v>
+        <v>0.002322939395445527</v>
       </c>
       <c r="P13" t="n">
-        <v>0.514711118492413</v>
+        <v>0.1707141036711313</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.452655709394133</v>
+        <v>0.4800000000214841</v>
       </c>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="n">
-        <v>0.01194494356088303</v>
+        <v>0.004857097145015834</v>
       </c>
       <c r="T13" t="n">
-        <v>0.2870982520990891</v>
+        <v>0.398237755523251</v>
       </c>
       <c r="U13" t="n">
-        <v>0.997227161030698</v>
+        <v>0.9971177963999001</v>
       </c>
       <c r="V13" t="n">
-        <v>0.9973553009761872</v>
+        <v>0.9971805700402812</v>
       </c>
       <c r="W13" t="n">
-        <v>72.79697065330559</v>
-      </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>Ne12</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>Ne12.txt</t>
-        </is>
+        <v>142.4794357250045</v>
+      </c>
+      <c r="X13" t="n">
+        <v>13.01017645999239</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>472.8263050090594</v>
       </c>
       <c r="Z13" t="inlineStr">
         <is>
+          <t>26 Ne12</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>26 Ne12.txt</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA13" t="inlineStr">
+      <c r="AC13" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB13" t="n">
+      <c r="AD13" t="n">
         <v>8</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AE13" t="n">
         <v>34.286</v>
       </c>
-      <c r="AD13" t="n">
+      <c r="AF13" t="n">
         <v>45</v>
       </c>
-      <c r="AE13" t="n">
+      <c r="AG13" t="n">
         <v>3</v>
       </c>
-      <c r="AF13" t="n">
+      <c r="AH13" t="n">
         <v>5</v>
       </c>
-      <c r="AG13" t="inlineStr">
+      <c r="AI13" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH13" t="inlineStr">
+      <c r="AJ13" t="inlineStr">
         <is>
           <t xml:space="preserve">2:19:10 PM
 </t>
         </is>
       </c>
-      <c r="AI13" t="n">
+      <c r="AK13" t="n">
         <v>51550</v>
       </c>
-      <c r="AJ13" t="n">
+      <c r="AL13" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -2080,119 +2162,125 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ne13.txt</t>
+          <t>29 Ne13.txt</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.9973014617895951</v>
+        <v>0.9971344221634375</v>
       </c>
       <c r="D14" t="n">
-        <v>4.684347899273643e-05</v>
+        <v>2.364363541008521e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>282.5907273689552</v>
+        <v>228.1108282995394</v>
       </c>
       <c r="F14" t="n">
-        <v>1399.226833417564</v>
+        <v>1447.924137648179</v>
       </c>
       <c r="G14" t="n">
-        <v>1116.636106048609</v>
+        <v>1219.81330934864</v>
       </c>
       <c r="H14" t="n">
-        <v>12239.95366711978</v>
+        <v>46610.37637817582</v>
       </c>
       <c r="I14" t="n">
-        <v>4390.629146197662</v>
+        <v>2601.675477863312</v>
       </c>
       <c r="J14" t="n">
-        <v>63.41213742559567</v>
+        <v>120.9991135020712</v>
       </c>
       <c r="K14" t="n">
-        <v>12.73141692227285</v>
+        <v>23.51097881779083</v>
       </c>
       <c r="L14" t="n">
-        <v>4.684347899273643e-05</v>
+        <v>2.364363541008521e-05</v>
       </c>
       <c r="M14" t="n">
-        <v>0.4418934346923539</v>
+        <v>0.4800000000092933</v>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>0.00644</v>
+        <v>0.002269819120386323</v>
       </c>
       <c r="P14" t="n">
-        <v>0.5308407463635317</v>
+        <v>0.1569368287217917</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.4526448387542288</v>
+        <v>0.4800000000015817</v>
       </c>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="n">
-        <v>0.01156540853834694</v>
+        <v>0.004892479239349929</v>
       </c>
       <c r="T14" t="n">
-        <v>0.2866084846395912</v>
+        <v>0.3946907298532736</v>
       </c>
       <c r="U14" t="n">
-        <v>0.9972379222801144</v>
+        <v>0.997103114793872</v>
       </c>
       <c r="V14" t="n">
-        <v>0.9973650093964944</v>
+        <v>0.9971657314990627</v>
       </c>
       <c r="W14" t="n">
-        <v>76.14355434786853</v>
-      </c>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>Ne13</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>Ne13.txt</t>
-        </is>
+        <v>144.5100923198621</v>
+      </c>
+      <c r="X14" t="n">
+        <v>254.2249808507208</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>481.8753874098571</v>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
+          <t>29 Ne13</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>29 Ne13.txt</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA14" t="inlineStr">
+      <c r="AC14" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB14" t="n">
+      <c r="AD14" t="n">
         <v>8</v>
       </c>
-      <c r="AC14" t="n">
+      <c r="AE14" t="n">
         <v>34.258</v>
       </c>
-      <c r="AD14" t="n">
+      <c r="AF14" t="n">
         <v>45</v>
       </c>
-      <c r="AE14" t="n">
+      <c r="AG14" t="n">
         <v>3</v>
       </c>
-      <c r="AF14" t="n">
+      <c r="AH14" t="n">
         <v>5</v>
       </c>
-      <c r="AG14" t="inlineStr">
+      <c r="AI14" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH14" t="inlineStr">
+      <c r="AJ14" t="inlineStr">
         <is>
           <t xml:space="preserve">2:35:24 PM
 </t>
         </is>
       </c>
-      <c r="AI14" t="n">
+      <c r="AK14" t="n">
         <v>52524</v>
       </c>
-      <c r="AJ14" t="n">
+      <c r="AL14" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -2202,119 +2290,125 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Ne14.txt</t>
+          <t>32 Ne14.txt</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.9972954149118481</v>
+        <v>0.9972153400075024</v>
       </c>
       <c r="D15" t="n">
-        <v>4.739733204635678e-05</v>
+        <v>7.368726641205315e-05</v>
       </c>
       <c r="E15" t="n">
-        <v>282.5924407946416</v>
+        <v>228.0923185196621</v>
       </c>
       <c r="F15" t="n">
-        <v>1399.223566201592</v>
+        <v>1447.920320866281</v>
       </c>
       <c r="G15" t="n">
-        <v>1116.63112540695</v>
+        <v>1219.828002346619</v>
       </c>
       <c r="H15" t="n">
-        <v>11608.22463653274</v>
+        <v>46068.86981891557</v>
       </c>
       <c r="I15" t="n">
-        <v>4405.567762634019</v>
+        <v>3158.663052725681</v>
       </c>
       <c r="J15" t="n">
-        <v>61.97233791162338</v>
+        <v>121.0043016392678</v>
       </c>
       <c r="K15" t="n">
-        <v>12.69226500986489</v>
+        <v>49.25024983213378</v>
       </c>
       <c r="L15" t="n">
-        <v>4.739733204635679e-05</v>
+        <v>7.368726641205315e-05</v>
       </c>
       <c r="M15" t="n">
-        <v>0.4421544918001505</v>
+        <v>0.480000000006112</v>
       </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>0.00661</v>
+        <v>0.002294921581421251</v>
       </c>
       <c r="P15" t="n">
-        <v>0.5343723301656037</v>
+        <v>0.1629458797466238</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.4552603177269076</v>
+        <v>0.4800000000070123</v>
       </c>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="n">
-        <v>0.01164948746455873</v>
+        <v>0.01665008625816899</v>
       </c>
       <c r="T15" t="n">
-        <v>0.2819955112336252</v>
+        <v>0.8307867756576435</v>
       </c>
       <c r="U15" t="n">
-        <v>0.997230979619381</v>
+        <v>0.9971325196673673</v>
       </c>
       <c r="V15" t="n">
-        <v>0.9973598585317245</v>
+        <v>0.9972981741066484</v>
       </c>
       <c r="W15" t="n">
-        <v>74.66460292148827</v>
-      </c>
-      <c r="X15" t="inlineStr">
-        <is>
-          <t>Ne14</t>
-        </is>
-      </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>Ne14.txt</t>
-        </is>
+        <v>170.2545514714016</v>
+      </c>
+      <c r="X15" t="n">
+        <v>117.6436666710624</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>480.2123420252391</v>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
+          <t>32 Ne14</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>32 Ne14.txt</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA15" t="inlineStr">
+      <c r="AC15" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB15" t="n">
+      <c r="AD15" t="n">
         <v>8</v>
       </c>
-      <c r="AC15" t="n">
+      <c r="AE15" t="n">
         <v>34.299</v>
       </c>
-      <c r="AD15" t="n">
+      <c r="AF15" t="n">
         <v>45</v>
       </c>
-      <c r="AE15" t="n">
+      <c r="AG15" t="n">
         <v>3</v>
       </c>
-      <c r="AF15" t="n">
+      <c r="AH15" t="n">
         <v>5</v>
       </c>
-      <c r="AG15" t="inlineStr">
+      <c r="AI15" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH15" t="inlineStr">
+      <c r="AJ15" t="inlineStr">
         <is>
           <t xml:space="preserve">2:44:47 PM
 </t>
         </is>
       </c>
-      <c r="AI15" t="n">
+      <c r="AK15" t="n">
         <v>53087</v>
       </c>
-      <c r="AJ15" t="n">
+      <c r="AL15" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -2324,119 +2418,125 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Ne15.txt</t>
+          <t>35 Ne15.txt</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.9973057223082753</v>
+        <v>0.9971125069633596</v>
       </c>
       <c r="D16" t="n">
-        <v>4.850578006369201e-05</v>
+        <v>2.407593957818995e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>282.5895201332542</v>
+        <v>228.1158418706332</v>
       </c>
       <c r="F16" t="n">
-        <v>1399.237991608165</v>
+        <v>1447.934255511347</v>
       </c>
       <c r="G16" t="n">
-        <v>1116.648471474911</v>
+        <v>1219.818413640714</v>
       </c>
       <c r="H16" t="n">
-        <v>12211.5025985104</v>
+        <v>47968.14381113181</v>
       </c>
       <c r="I16" t="n">
-        <v>4364.60872910606</v>
+        <v>2670.322540783967</v>
       </c>
       <c r="J16" t="n">
-        <v>63.76441691638503</v>
+        <v>121.8315702467341</v>
       </c>
       <c r="K16" t="n">
-        <v>13.84711154172536</v>
+        <v>23.35975048696288</v>
       </c>
       <c r="L16" t="n">
-        <v>4.8505780063692e-05</v>
+        <v>2.407593957818995e-05</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4414397011627023</v>
+        <v>0.4800000000168914</v>
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.00647</v>
+        <v>0.002214930383247553</v>
       </c>
       <c r="P16" t="n">
-        <v>0.5367213038163581</v>
+        <v>0.1563914001675262</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.4581124363034833</v>
+        <v>0.480000000083708</v>
       </c>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
-        <v>0.01208416816615732</v>
+        <v>0.005025662268713386</v>
       </c>
       <c r="T16" t="n">
-        <v>0.3044435860585134</v>
+        <v>0.3913796148926349</v>
       </c>
       <c r="U16" t="n">
-        <v>0.9972402458418629</v>
+        <v>0.9970808587609371</v>
       </c>
       <c r="V16" t="n">
-        <v>0.9973712073733161</v>
+        <v>0.997144157174928</v>
       </c>
       <c r="W16" t="n">
-        <v>77.61152845811039</v>
-      </c>
-      <c r="X16" t="inlineStr">
-        <is>
-          <t>Ne15</t>
-        </is>
-      </c>
-      <c r="Y16" t="inlineStr">
-        <is>
-          <t>Ne15.txt</t>
-        </is>
+        <v>145.191320733697</v>
+      </c>
+      <c r="X16" t="n">
+        <v>110.0754584717833</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>483.125322925331</v>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
+          <t>35 Ne15</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>35 Ne15.txt</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA16" t="inlineStr">
+      <c r="AC16" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB16" t="n">
+      <c r="AD16" t="n">
         <v>8</v>
       </c>
-      <c r="AC16" t="n">
+      <c r="AE16" t="n">
         <v>34.109</v>
       </c>
-      <c r="AD16" t="n">
+      <c r="AF16" t="n">
         <v>45</v>
       </c>
-      <c r="AE16" t="n">
+      <c r="AG16" t="n">
         <v>3</v>
       </c>
-      <c r="AF16" t="n">
+      <c r="AH16" t="n">
         <v>5</v>
       </c>
-      <c r="AG16" t="inlineStr">
+      <c r="AI16" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH16" t="inlineStr">
+      <c r="AJ16" t="inlineStr">
         <is>
           <t xml:space="preserve">2:56:55 PM
 </t>
         </is>
       </c>
-      <c r="AI16" t="n">
+      <c r="AK16" t="n">
         <v>53815</v>
       </c>
-      <c r="AJ16" t="n">
+      <c r="AL16" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -2446,119 +2546,125 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ne16.txt</t>
+          <t>37 Ne16.txt</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.997296179471089</v>
+        <v>0.9971251510770303</v>
       </c>
       <c r="D17" t="n">
-        <v>4.77464293650123e-05</v>
+        <v>2.360495987818484e-05</v>
       </c>
       <c r="E17" t="n">
-        <v>282.5922241502119</v>
+        <v>228.1129492320997</v>
       </c>
       <c r="F17" t="n">
-        <v>1399.243120855637</v>
+        <v>1447.938607854202</v>
       </c>
       <c r="G17" t="n">
-        <v>1116.650896705425</v>
+        <v>1219.825658622102</v>
       </c>
       <c r="H17" t="n">
-        <v>12061.55275240272</v>
+        <v>49604.62513716722</v>
       </c>
       <c r="I17" t="n">
-        <v>4312.397931425139</v>
+        <v>2696.725059566181</v>
       </c>
       <c r="J17" t="n">
-        <v>63.684445722832</v>
+        <v>126.1431357296601</v>
       </c>
       <c r="K17" t="n">
-        <v>11.78949190803532</v>
+        <v>24.67964014876316</v>
       </c>
       <c r="L17" t="n">
-        <v>4.774642936501231e-05</v>
+        <v>2.360495987818484e-05</v>
       </c>
       <c r="M17" t="n">
-        <v>0.4444428583730871</v>
+        <v>0.4800000000141028</v>
       </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>0.00656</v>
+        <v>0.002205793157936598</v>
       </c>
       <c r="P17" t="n">
-        <v>0.5388377793482646</v>
+        <v>0.1603839815864463</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.452228350191162</v>
+        <v>0.4800000000007883</v>
       </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="n">
-        <v>0.01179072658295087</v>
+        <v>0.004912062861059882</v>
       </c>
       <c r="T17" t="n">
-        <v>0.2994334475551614</v>
+        <v>0.3662542642804673</v>
       </c>
       <c r="U17" t="n">
-        <v>0.9972314221295783</v>
+        <v>0.9970940385434041</v>
       </c>
       <c r="V17" t="n">
-        <v>0.9973609452234571</v>
+        <v>0.9971562655523388</v>
       </c>
       <c r="W17" t="n">
-        <v>75.47393763086731</v>
-      </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>Ne16</t>
-        </is>
-      </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>Ne16.txt</t>
-        </is>
+        <v>150.8227758784233</v>
+      </c>
+      <c r="X17" t="n">
+        <v>40.3224985446176</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>495.6797850427561</v>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
+          <t>37 Ne16</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>37 Ne16.txt</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA17" t="inlineStr">
+      <c r="AC17" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB17" t="n">
+      <c r="AD17" t="n">
         <v>8</v>
       </c>
-      <c r="AC17" t="n">
+      <c r="AE17" t="n">
         <v>34.113</v>
       </c>
-      <c r="AD17" t="n">
+      <c r="AF17" t="n">
         <v>45</v>
       </c>
-      <c r="AE17" t="n">
+      <c r="AG17" t="n">
         <v>3</v>
       </c>
-      <c r="AF17" t="n">
+      <c r="AH17" t="n">
         <v>5</v>
       </c>
-      <c r="AG17" t="inlineStr">
+      <c r="AI17" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH17" t="inlineStr">
+      <c r="AJ17" t="inlineStr">
         <is>
           <t xml:space="preserve">3:03:54 PM
 </t>
         </is>
       </c>
-      <c r="AI17" t="n">
+      <c r="AK17" t="n">
         <v>54234</v>
       </c>
-      <c r="AJ17" t="n">
+      <c r="AL17" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -2568,119 +2674,125 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ne17.txt</t>
+          <t>41 Ne17.txt</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.9972807148676196</v>
+        <v>0.9971298762293466</v>
       </c>
       <c r="D18" t="n">
-        <v>4.74824412203751e-05</v>
+        <v>2.383797877471338e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>282.5966062430618</v>
+        <v>228.1118682611489</v>
       </c>
       <c r="F18" t="n">
-        <v>1399.236738631383</v>
+        <v>1447.931707502355</v>
       </c>
       <c r="G18" t="n">
-        <v>1116.640132388321</v>
+        <v>1219.819839241206</v>
       </c>
       <c r="H18" t="n">
-        <v>11966.5585971399</v>
+        <v>46387.26704286027</v>
       </c>
       <c r="I18" t="n">
-        <v>4326.803771491455</v>
+        <v>2707.285989420517</v>
       </c>
       <c r="J18" t="n">
-        <v>62.40242798962629</v>
+        <v>114.6423382685321</v>
       </c>
       <c r="K18" t="n">
-        <v>12.70769554232494</v>
+        <v>22.89143644071131</v>
       </c>
       <c r="L18" t="n">
-        <v>4.748244122037509e-05</v>
+        <v>2.383797877471338e-05</v>
       </c>
       <c r="M18" t="n">
-        <v>0.4438444950822464</v>
+        <v>0.4800000000000056</v>
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>0.00655</v>
+        <v>0.002237624038393856</v>
       </c>
       <c r="P18" t="n">
-        <v>0.5376343380182946</v>
+        <v>0.1764008642662193</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.4526246723041308</v>
+        <v>0.4800000000008278</v>
       </c>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="n">
-        <v>0.01171112012025851</v>
+        <v>0.004955996503444244</v>
       </c>
       <c r="T18" t="n">
-        <v>0.2936606244318223</v>
+        <v>0.386103473887326</v>
       </c>
       <c r="U18" t="n">
-        <v>0.9972162757137358</v>
+        <v>0.9970984322373306</v>
       </c>
       <c r="V18" t="n">
-        <v>0.9973451623500336</v>
+        <v>0.9971613222046286</v>
       </c>
       <c r="W18" t="n">
-        <v>75.11012353195123</v>
-      </c>
-      <c r="X18" t="inlineStr">
-        <is>
-          <t>Ne17</t>
-        </is>
-      </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>Ne17.txt</t>
-        </is>
+        <v>137.5337747092434</v>
+      </c>
+      <c r="X18" t="n">
+        <v>21.90559390996007</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>469.0516097453981</v>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
+          <t>41 Ne17</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>41 Ne17.txt</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA18" t="inlineStr">
+      <c r="AC18" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB18" t="n">
+      <c r="AD18" t="n">
         <v>8</v>
       </c>
-      <c r="AC18" t="n">
+      <c r="AE18" t="n">
         <v>34.136</v>
       </c>
-      <c r="AD18" t="n">
+      <c r="AF18" t="n">
         <v>45</v>
       </c>
-      <c r="AE18" t="n">
+      <c r="AG18" t="n">
         <v>3</v>
       </c>
-      <c r="AF18" t="n">
+      <c r="AH18" t="n">
         <v>5</v>
       </c>
-      <c r="AG18" t="inlineStr">
+      <c r="AI18" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH18" t="inlineStr">
+      <c r="AJ18" t="inlineStr">
         <is>
           <t xml:space="preserve">3:21:55 PM
 </t>
         </is>
       </c>
-      <c r="AI18" t="n">
+      <c r="AK18" t="n">
         <v>55315</v>
       </c>
-      <c r="AJ18" t="n">
+      <c r="AL18" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -2690,119 +2802,125 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Ne18.txt</t>
+          <t>43 Ne18.txt</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.9972858096584727</v>
+        <v>0.9971555646094575</v>
       </c>
       <c r="D19" t="n">
-        <v>4.931039328179225e-05</v>
+        <v>2.180196030528756e-05</v>
       </c>
       <c r="E19" t="n">
-        <v>282.5951625540104</v>
+        <v>228.1059917213313</v>
       </c>
       <c r="F19" t="n">
-        <v>1399.240458026143</v>
+        <v>1447.940548166711</v>
       </c>
       <c r="G19" t="n">
-        <v>1116.645295472132</v>
+        <v>1219.834556445379</v>
       </c>
       <c r="H19" t="n">
-        <v>12341.20334816642</v>
+        <v>47084.98019026718</v>
       </c>
       <c r="I19" t="n">
-        <v>4261.379807456812</v>
+        <v>2564.305636927529</v>
       </c>
       <c r="J19" t="n">
-        <v>64.61912943879629</v>
+        <v>116.9733922133446</v>
       </c>
       <c r="K19" t="n">
-        <v>12.2927651473398</v>
+        <v>21.51775839661121</v>
       </c>
       <c r="L19" t="n">
-        <v>4.931039328179225e-05</v>
+        <v>2.180196030528756e-05</v>
       </c>
       <c r="M19" t="n">
-        <v>0.4420997128472524</v>
+        <v>0.4800000000038325</v>
       </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>0.00658</v>
+        <v>0.002203918126226992</v>
       </c>
       <c r="P19" t="n">
-        <v>0.5338212390098799</v>
+        <v>0.1752415289755787</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.454936030898626</v>
+        <v>0.4800000001048549</v>
       </c>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="n">
-        <v>0.01228350282851129</v>
+        <v>0.004458143466387759</v>
       </c>
       <c r="T19" t="n">
-        <v>0.3044979388504679</v>
+        <v>0.3395383419469948</v>
       </c>
       <c r="U19" t="n">
-        <v>0.9972192443009292</v>
+        <v>0.9971264425433265</v>
       </c>
       <c r="V19" t="n">
-        <v>0.9973523839032147</v>
+        <v>0.9971846883767159</v>
       </c>
       <c r="W19" t="n">
-        <v>76.9118945861361</v>
-      </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t>Ne18</t>
-        </is>
-      </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>Ne18.txt</t>
-        </is>
+        <v>138.4911506099558</v>
+      </c>
+      <c r="X19" t="n">
+        <v>9.512308940311035</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>466.9638940678363</v>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
+          <t>43 Ne18</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>43 Ne18.txt</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA19" t="inlineStr">
+      <c r="AC19" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB19" t="n">
+      <c r="AD19" t="n">
         <v>8</v>
       </c>
-      <c r="AC19" t="n">
+      <c r="AE19" t="n">
         <v>34.042</v>
       </c>
-      <c r="AD19" t="n">
+      <c r="AF19" t="n">
         <v>45</v>
       </c>
-      <c r="AE19" t="n">
+      <c r="AG19" t="n">
         <v>3</v>
       </c>
-      <c r="AF19" t="n">
+      <c r="AH19" t="n">
         <v>5</v>
       </c>
-      <c r="AG19" t="inlineStr">
+      <c r="AI19" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH19" t="inlineStr">
+      <c r="AJ19" t="inlineStr">
         <is>
           <t xml:space="preserve">3:31:59 PM
 </t>
         </is>
       </c>
-      <c r="AI19" t="n">
+      <c r="AK19" t="n">
         <v>55919</v>
       </c>
-      <c r="AJ19" t="n">
+      <c r="AL19" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -2812,119 +2930,125 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ne19.txt</t>
+          <t>45 Ne19.txt</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.9972848521456855</v>
+        <v>0.9971275671903285</v>
       </c>
       <c r="D20" t="n">
-        <v>4.886401020447739e-05</v>
+        <v>2.176781150978165e-05</v>
       </c>
       <c r="E20" t="n">
-        <v>282.5954338791801</v>
+        <v>228.1123964976771</v>
       </c>
       <c r="F20" t="n">
-        <v>1399.254872650147</v>
+        <v>1447.95428924492</v>
       </c>
       <c r="G20" t="n">
-        <v>1116.659438770967</v>
+        <v>1219.841892747243</v>
       </c>
       <c r="H20" t="n">
-        <v>12588.64683132001</v>
+        <v>47151.24770158556</v>
       </c>
       <c r="I20" t="n">
-        <v>4241.197337490735</v>
+        <v>2638.639174448726</v>
       </c>
       <c r="J20" t="n">
-        <v>64.6451949172981</v>
+        <v>116.9054207933831</v>
       </c>
       <c r="K20" t="n">
-        <v>11.84960753812245</v>
+        <v>22.81094608042548</v>
       </c>
       <c r="L20" t="n">
-        <v>4.886401020447739e-05</v>
+        <v>2.176781150978165e-05</v>
       </c>
       <c r="M20" t="n">
-        <v>0.4390589410827008</v>
+        <v>0.4800000000001555</v>
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>0.00655</v>
+        <v>0.00224037153276129</v>
       </c>
       <c r="P20" t="n">
-        <v>0.551050257230309</v>
+        <v>0.1810162210767646</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.4534045207368897</v>
+        <v>0.4800000000182647</v>
       </c>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="n">
-        <v>0.01215643741579669</v>
+        <v>0.004431365660545409</v>
       </c>
       <c r="T20" t="n">
-        <v>0.3002063619988237</v>
+        <v>0.3203675763067519</v>
       </c>
       <c r="U20" t="n">
-        <v>0.9972188411292108</v>
+        <v>0.9970984044678609</v>
       </c>
       <c r="V20" t="n">
-        <v>0.9973508719019526</v>
+        <v>0.9971567316187244</v>
       </c>
       <c r="W20" t="n">
-        <v>76.49480245542055</v>
-      </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>Ne19</t>
-        </is>
-      </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>Ne19.txt</t>
-        </is>
+        <v>139.7163668738085</v>
+      </c>
+      <c r="X20" t="n">
+        <v>34.52460675594876</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>467.7447740971828</v>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
+          <t>45 Ne19</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>45 Ne19.txt</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA20" t="inlineStr">
+      <c r="AC20" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB20" t="n">
+      <c r="AD20" t="n">
         <v>8</v>
       </c>
-      <c r="AC20" t="n">
+      <c r="AE20" t="n">
         <v>33.904</v>
       </c>
-      <c r="AD20" t="n">
+      <c r="AF20" t="n">
         <v>45</v>
       </c>
-      <c r="AE20" t="n">
+      <c r="AG20" t="n">
         <v>3</v>
       </c>
-      <c r="AF20" t="n">
+      <c r="AH20" t="n">
         <v>5</v>
       </c>
-      <c r="AG20" t="inlineStr">
+      <c r="AI20" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH20" t="inlineStr">
+      <c r="AJ20" t="inlineStr">
         <is>
           <t xml:space="preserve">3:41:07 PM
 </t>
         </is>
       </c>
-      <c r="AI20" t="n">
+      <c r="AK20" t="n">
         <v>56467</v>
       </c>
-      <c r="AJ20" t="n">
+      <c r="AL20" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -2934,119 +3058,125 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Ne20.txt</t>
+          <t>50 Ne20.txt</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.9972818376306362</v>
+        <v>0.9971305309945541</v>
       </c>
       <c r="D21" t="n">
-        <v>4.575113656610273e-05</v>
+        <v>2.214513293775388e-05</v>
       </c>
       <c r="E21" t="n">
-        <v>282.59628808925</v>
+        <v>228.1117184716177</v>
       </c>
       <c r="F21" t="n">
-        <v>1399.241745145151</v>
+        <v>1447.938544984182</v>
       </c>
       <c r="G21" t="n">
-        <v>1116.645457055901</v>
+        <v>1219.826826512565</v>
       </c>
       <c r="H21" t="n">
-        <v>11945.31065045132</v>
+        <v>46554.29067845942</v>
       </c>
       <c r="I21" t="n">
-        <v>4491.164396086388</v>
+        <v>2600.863287229956</v>
       </c>
       <c r="J21" t="n">
-        <v>61.8583615987184</v>
+        <v>116.8588540735299</v>
       </c>
       <c r="K21" t="n">
-        <v>12.69350079877464</v>
+        <v>21.2925895535408</v>
       </c>
       <c r="L21" t="n">
-        <v>4.575113656610273e-05</v>
+        <v>2.214513293775388e-05</v>
       </c>
       <c r="M21" t="n">
-        <v>0.4428187163957512</v>
+        <v>0.4800000000105936</v>
       </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>0.00643</v>
+        <v>0.002236487123594576</v>
       </c>
       <c r="P21" t="n">
-        <v>0.5322288175086354</v>
+        <v>0.1749382155684411</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.4583006832229925</v>
+        <v>0.4800000000016865</v>
       </c>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="n">
-        <v>0.01121680713132682</v>
+        <v>0.004529506322799496</v>
       </c>
       <c r="T21" t="n">
-        <v>0.2705447465282427</v>
+        <v>0.3675078248273268</v>
       </c>
       <c r="U21" t="n">
-        <v>0.9972195659657563</v>
+        <v>0.9971009561065141</v>
       </c>
       <c r="V21" t="n">
-        <v>0.997344117073146</v>
+        <v>0.9971601076370802</v>
       </c>
       <c r="W21" t="n">
-        <v>74.55186239749304</v>
-      </c>
-      <c r="X21" t="inlineStr">
-        <is>
-          <t>Ne20</t>
-        </is>
-      </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>Ne20.txt</t>
-        </is>
+        <v>138.1514436270707</v>
+      </c>
+      <c r="X21" t="n">
+        <v>70.60910859120509</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>469.2245087910743</v>
       </c>
       <c r="Z21" t="inlineStr">
         <is>
+          <t>50 Ne20</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>50 Ne20.txt</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA21" t="inlineStr">
+      <c r="AC21" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB21" t="n">
+      <c r="AD21" t="n">
         <v>8</v>
       </c>
-      <c r="AC21" t="n">
+      <c r="AE21" t="n">
         <v>34.006</v>
       </c>
-      <c r="AD21" t="n">
+      <c r="AF21" t="n">
         <v>45</v>
       </c>
-      <c r="AE21" t="n">
+      <c r="AG21" t="n">
         <v>3</v>
       </c>
-      <c r="AF21" t="n">
+      <c r="AH21" t="n">
         <v>5</v>
       </c>
-      <c r="AG21" t="inlineStr">
+      <c r="AI21" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH21" t="inlineStr">
+      <c r="AJ21" t="inlineStr">
         <is>
           <t xml:space="preserve">4:04:08 PM
 </t>
         </is>
       </c>
-      <c r="AI21" t="n">
+      <c r="AK21" t="n">
         <v>57848</v>
       </c>
-      <c r="AJ21" t="n">
+      <c r="AL21" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -3056,119 +3186,125 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ne21.txt</t>
+          <t>54 Ne21.txt</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.9972854055576105</v>
+        <v>0.9971399578210725</v>
       </c>
       <c r="D22" t="n">
-        <v>4.7822662750829e-05</v>
+        <v>2.173665140519148e-05</v>
       </c>
       <c r="E22" t="n">
-        <v>282.5952770618014</v>
+        <v>228.1095619342329</v>
       </c>
       <c r="F22" t="n">
-        <v>1399.250988594828</v>
+        <v>1447.949609029153</v>
       </c>
       <c r="G22" t="n">
-        <v>1116.655711533027</v>
+        <v>1219.84004709492</v>
       </c>
       <c r="H22" t="n">
-        <v>12570.17418707135</v>
+        <v>47535.00685786141</v>
       </c>
       <c r="I22" t="n">
-        <v>4334.56264216619</v>
+        <v>2668.291470408012</v>
       </c>
       <c r="J22" t="n">
-        <v>64.63026964183287</v>
+        <v>113.9799629230929</v>
       </c>
       <c r="K22" t="n">
-        <v>11.78493067850383</v>
+        <v>22.20134228620324</v>
       </c>
       <c r="L22" t="n">
-        <v>4.7822662750829e-05</v>
+        <v>2.173665140519148e-05</v>
       </c>
       <c r="M22" t="n">
-        <v>0.4427201375812689</v>
+        <v>0.4800000000002652</v>
       </c>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>0.00637</v>
+        <v>0.002190361505238868</v>
       </c>
       <c r="P22" t="n">
-        <v>0.5334385110472623</v>
+        <v>0.1788297148279032</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.4545502569420428</v>
+        <v>0.4800000000140576</v>
       </c>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="n">
-        <v>0.01191904744765186</v>
+        <v>0.00444830669982065</v>
       </c>
       <c r="T22" t="n">
-        <v>0.2999380291050648</v>
+        <v>0.3317747696545701</v>
       </c>
       <c r="U22" t="n">
-        <v>0.9972208672541161</v>
+        <v>0.9971109389205457</v>
       </c>
       <c r="V22" t="n">
-        <v>0.9973499522152466</v>
+        <v>0.9971689784107215</v>
       </c>
       <c r="W22" t="n">
-        <v>76.41520032033669</v>
-      </c>
-      <c r="X22" t="inlineStr">
-        <is>
-          <t>Ne21</t>
-        </is>
-      </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>Ne21.txt</t>
-        </is>
+        <v>136.1813052092962</v>
+      </c>
+      <c r="X22" t="n">
+        <v>29.46354514586258</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>464.000593751266</v>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
+          <t>54 Ne21</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>54 Ne21.txt</t>
+        </is>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA22" t="inlineStr">
+      <c r="AC22" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB22" t="n">
+      <c r="AD22" t="n">
         <v>8</v>
       </c>
-      <c r="AC22" t="n">
+      <c r="AE22" t="n">
         <v>33.911</v>
       </c>
-      <c r="AD22" t="n">
+      <c r="AF22" t="n">
         <v>45</v>
       </c>
-      <c r="AE22" t="n">
+      <c r="AG22" t="n">
         <v>3</v>
       </c>
-      <c r="AF22" t="n">
+      <c r="AH22" t="n">
         <v>5</v>
       </c>
-      <c r="AG22" t="inlineStr">
+      <c r="AI22" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH22" t="inlineStr">
+      <c r="AJ22" t="inlineStr">
         <is>
           <t xml:space="preserve">4:32:25 PM
 </t>
         </is>
       </c>
-      <c r="AI22" t="n">
+      <c r="AK22" t="n">
         <v>59545</v>
       </c>
-      <c r="AJ22" t="n">
+      <c r="AL22" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -3178,119 +3314,125 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ne22.txt</t>
+          <t>57 Ne22.txt</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.9972741265988673</v>
+        <v>0.9971414675941587</v>
       </c>
       <c r="D23" t="n">
-        <v>4.732820636453446e-05</v>
+        <v>2.152238828137372e-05</v>
       </c>
       <c r="E23" t="n">
-        <v>282.5984731544163</v>
+        <v>228.109216553273</v>
       </c>
       <c r="F23" t="n">
-        <v>1399.245588212064</v>
+        <v>1447.941180640094</v>
       </c>
       <c r="G23" t="n">
-        <v>1116.647115057648</v>
+        <v>1219.831964086821</v>
       </c>
       <c r="H23" t="n">
-        <v>12465.43223888202</v>
+        <v>46263.90003460313</v>
       </c>
       <c r="I23" t="n">
-        <v>4342.401014243318</v>
+        <v>2631.327655112118</v>
       </c>
       <c r="J23" t="n">
-        <v>65.05631766903154</v>
+        <v>112.7724518600126</v>
       </c>
       <c r="K23" t="n">
-        <v>12.76657447945282</v>
+        <v>22.20215776937436</v>
       </c>
       <c r="L23" t="n">
-        <v>4.732820636453445e-05</v>
+        <v>2.152238828137372e-05</v>
       </c>
       <c r="M23" t="n">
-        <v>0.4454715012013401</v>
+        <v>0.4800000000027006</v>
       </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>0.00653</v>
+        <v>0.002216545869630283</v>
       </c>
       <c r="P23" t="n">
-        <v>0.539257172661317</v>
+        <v>0.1794330442924574</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.457010634140955</v>
+        <v>0.4800000000142952</v>
       </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="n">
-        <v>0.01167246693746059</v>
+        <v>0.004380602021828121</v>
       </c>
       <c r="T23" t="n">
-        <v>0.2799606137618459</v>
+        <v>0.3462714456215095</v>
       </c>
       <c r="U23" t="n">
-        <v>0.997209895253434</v>
+        <v>0.9971126300943648</v>
       </c>
       <c r="V23" t="n">
-        <v>0.9973383662192515</v>
+        <v>0.9971703067620198</v>
       </c>
       <c r="W23" t="n">
-        <v>77.82289214848436</v>
-      </c>
-      <c r="X23" t="inlineStr">
-        <is>
-          <t>Ne22</t>
-        </is>
-      </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>Ne22.txt</t>
-        </is>
+        <v>134.974609629387</v>
+      </c>
+      <c r="X23" t="n">
+        <v>31.63782391314893</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>460.5273874291144</v>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
+          <t>57 Ne22</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>57 Ne22.txt</t>
+        </is>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA23" t="inlineStr">
+      <c r="AC23" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB23" t="n">
+      <c r="AD23" t="n">
         <v>8</v>
       </c>
-      <c r="AC23" t="n">
+      <c r="AE23" t="n">
         <v>33.96</v>
       </c>
-      <c r="AD23" t="n">
+      <c r="AF23" t="n">
         <v>45</v>
       </c>
-      <c r="AE23" t="n">
+      <c r="AG23" t="n">
         <v>3</v>
       </c>
-      <c r="AF23" t="n">
+      <c r="AH23" t="n">
         <v>5</v>
       </c>
-      <c r="AG23" t="inlineStr">
+      <c r="AI23" t="inlineStr">
         <is>
           <t>['0h', '2m', '17s']</t>
         </is>
       </c>
-      <c r="AH23" t="inlineStr">
+      <c r="AJ23" t="inlineStr">
         <is>
           <t xml:space="preserve">4:44:38 PM
 </t>
         </is>
       </c>
-      <c r="AI23" t="n">
+      <c r="AK23" t="n">
         <v>60278</v>
       </c>
-      <c r="AJ23" t="n">
+      <c r="AL23" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -3300,119 +3442,125 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Ne23.txt</t>
+          <t>59 Ne23.txt</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.997270885596346</v>
+        <v>0.9971298718500308</v>
       </c>
       <c r="D24" t="n">
-        <v>4.574758196571692e-05</v>
+        <v>2.190290037516799e-05</v>
       </c>
       <c r="E24" t="n">
-        <v>282.599391563223</v>
+        <v>228.1118692629982</v>
       </c>
       <c r="F24" t="n">
-        <v>1399.245127792242</v>
+        <v>1447.942889094987</v>
       </c>
       <c r="G24" t="n">
-        <v>1116.645736229019</v>
+        <v>1219.831019831988</v>
       </c>
       <c r="H24" t="n">
-        <v>12301.47505613598</v>
+        <v>47482.27582250073</v>
       </c>
       <c r="I24" t="n">
-        <v>4460.268201046609</v>
+        <v>2599.238475568886</v>
       </c>
       <c r="J24" t="n">
-        <v>62.61583338903288</v>
+        <v>112.9523196500019</v>
       </c>
       <c r="K24" t="n">
-        <v>13.07598597480066</v>
+        <v>21.37775032391121</v>
       </c>
       <c r="L24" t="n">
-        <v>4.574758196571692e-05</v>
+        <v>2.190290037516799e-05</v>
       </c>
       <c r="M24" t="n">
-        <v>0.4421198263438217</v>
+        <v>0.4800000000002864</v>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>0.0062</v>
+        <v>0.002190300757714609</v>
       </c>
       <c r="P24" t="n">
-        <v>0.5293258107604308</v>
+        <v>0.1799982886544438</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.4541008147507578</v>
+        <v>0.4800000001293425</v>
       </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="n">
-        <v>0.01134457399903894</v>
+        <v>0.004490624863429288</v>
       </c>
       <c r="T24" t="n">
-        <v>0.3044351938707684</v>
+        <v>0.3459013399323216</v>
       </c>
       <c r="U24" t="n">
-        <v>0.9972089760268471</v>
+        <v>0.9971006688303599</v>
       </c>
       <c r="V24" t="n">
-        <v>0.9973328028533666</v>
+        <v>0.997159076580344</v>
       </c>
       <c r="W24" t="n">
-        <v>75.69181936383353</v>
-      </c>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>Ne23</t>
-        </is>
-      </c>
-      <c r="Y24" t="inlineStr">
-        <is>
-          <t>Ne23.txt</t>
-        </is>
+        <v>134.3300699739131</v>
+      </c>
+      <c r="X24" t="n">
+        <v>30.03522680753089</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>466.3309540250446</v>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
+          <t>59 Ne23</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>59 Ne23.txt</t>
+        </is>
+      </c>
+      <c r="AB24" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA24" t="inlineStr">
+      <c r="AC24" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB24" t="n">
+      <c r="AD24" t="n">
         <v>8</v>
       </c>
-      <c r="AC24" t="n">
+      <c r="AE24" t="n">
         <v>34.005</v>
       </c>
-      <c r="AD24" t="n">
+      <c r="AF24" t="n">
         <v>45</v>
       </c>
-      <c r="AE24" t="n">
+      <c r="AG24" t="n">
         <v>3</v>
       </c>
-      <c r="AF24" t="n">
+      <c r="AH24" t="n">
         <v>5</v>
       </c>
-      <c r="AG24" t="inlineStr">
+      <c r="AI24" t="inlineStr">
         <is>
           <t>['0h', '2m', '16s']</t>
         </is>
       </c>
-      <c r="AH24" t="inlineStr">
+      <c r="AJ24" t="inlineStr">
         <is>
           <t xml:space="preserve">5:21:49 PM
 </t>
         </is>
       </c>
-      <c r="AI24" t="n">
+      <c r="AK24" t="n">
         <v>62509</v>
       </c>
-      <c r="AJ24" t="n">
+      <c r="AL24" t="n">
         <v>1325.004</v>
       </c>
     </row>
@@ -3422,119 +3570,125 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ne24.txt</t>
+          <t>60 Ne24.txt</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.9972842751195219</v>
+        <v>0.9971156179327674</v>
       </c>
       <c r="D25" t="n">
-        <v>4.921111949400546e-05</v>
+        <v>2.262738769515692e-05</v>
       </c>
       <c r="E25" t="n">
-        <v>282.5955973881846</v>
+        <v>228.1151301563718</v>
       </c>
       <c r="F25" t="n">
-        <v>1399.242967921819</v>
+        <v>1447.942056897386</v>
       </c>
       <c r="G25" t="n">
-        <v>1116.647370533634</v>
+        <v>1219.826926741014</v>
       </c>
       <c r="H25" t="n">
-        <v>12026.79712582903</v>
+        <v>45197.53089639871</v>
       </c>
       <c r="I25" t="n">
-        <v>4101.153869931458</v>
+        <v>2652.856054907274</v>
       </c>
       <c r="J25" t="n">
-        <v>60.97468052180886</v>
+        <v>111.9819577169404</v>
       </c>
       <c r="K25" t="n">
-        <v>12.94010960149286</v>
+        <v>22.04734986376765</v>
       </c>
       <c r="L25" t="n">
-        <v>4.921111949400547e-05</v>
+        <v>2.262738769515692e-05</v>
       </c>
       <c r="M25" t="n">
-        <v>0.443546717952081</v>
+        <v>0.4800000000020138</v>
       </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>0.00623</v>
+        <v>0.002274139127232912</v>
       </c>
       <c r="P25" t="n">
-        <v>0.5264437827670779</v>
+        <v>0.1840672534173819</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.4497923104267718</v>
+        <v>0.4800000000016393</v>
       </c>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="n">
-        <v>0.0124333204593484</v>
+        <v>0.004633672051314634</v>
       </c>
       <c r="T25" t="n">
-        <v>0.3093050558151199</v>
+        <v>0.363470239712105</v>
       </c>
       <c r="U25" t="n">
-        <v>0.9972184163197253</v>
+        <v>0.9970854240660406</v>
       </c>
       <c r="V25" t="n">
-        <v>0.9973501426188528</v>
+        <v>0.9971458136282184</v>
       </c>
       <c r="W25" t="n">
-        <v>73.91479012330173</v>
-      </c>
-      <c r="X25" t="inlineStr">
-        <is>
-          <t>Ne24</t>
-        </is>
-      </c>
-      <c r="Y25" t="inlineStr">
-        <is>
-          <t>Ne24.txt</t>
-        </is>
+        <v>134.0293075807081</v>
+      </c>
+      <c r="X25" t="n">
+        <v>88.48553175384347</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>460.5108901060727</v>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
+          <t>60 Ne24</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>60 Ne24.txt</t>
+        </is>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
           <t xml:space="preserve">June 8, 2023
 </t>
         </is>
       </c>
-      <c r="AA25" t="inlineStr">
+      <c r="AC25" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="AB25" t="n">
+      <c r="AD25" t="n">
         <v>8</v>
       </c>
-      <c r="AC25" t="n">
+      <c r="AE25" t="n">
         <v>0</v>
       </c>
-      <c r="AD25" t="n">
+      <c r="AF25" t="n">
         <v>45</v>
       </c>
-      <c r="AE25" t="n">
+      <c r="AG25" t="n">
         <v>3</v>
       </c>
-      <c r="AF25" t="n">
+      <c r="AH25" t="n">
         <v>5</v>
       </c>
-      <c r="AG25" t="inlineStr">
+      <c r="AI25" t="inlineStr">
         <is>
           <t>['0h', '2m', '16s']</t>
         </is>
       </c>
-      <c r="AH25" t="inlineStr">
+      <c r="AJ25" t="inlineStr">
         <is>
           <t xml:space="preserve">5:24:27 PM
 </t>
         </is>
       </c>
-      <c r="AI25" t="n">
+      <c r="AK25" t="n">
         <v>62667</v>
       </c>
-      <c r="AJ25" t="n">
+      <c r="AL25" t="n">
         <v>1325.004</v>
       </c>
     </row>

</xml_diff>